<commit_message>
Initial Adaptation to Economy Update
Removed backwards compatibility with older versions and obscure mods as well. Probably overkilled it a little, but here goes trying!
</commit_message>
<xml_diff>
--- a/Detailed Ore Data.xlsx
+++ b/Detailed Ore Data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drank\AppData\Roaming\SpaceEngineers\Mods\DranKofBetterStone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06A79E1-618F-4471-8DEB-D909A488C58A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AEABA1-81A9-40C0-919F-71006A5E3C97}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Processing Speeds" sheetId="2" r:id="rId1"/>
-    <sheet name="Distributions" sheetId="1" r:id="rId2"/>
+    <sheet name="ECON UPDATE" sheetId="3" r:id="rId1"/>
+    <sheet name="Processing Speeds" sheetId="2" r:id="rId2"/>
+    <sheet name="Distributions" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="142">
   <si>
     <t>Ore Input:Output Ratios</t>
   </si>
@@ -504,6 +505,39 @@
   </si>
   <si>
     <t>S (CM)</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>Min,PerUnit</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min,Acqu</t>
+  </si>
+  <si>
+    <t>Max,Acqu</t>
+  </si>
+  <si>
+    <t>Max Also ?:</t>
+  </si>
+  <si>
+    <t>Interpreted Tier</t>
+  </si>
+  <si>
+    <t>Should be 300</t>
+  </si>
+  <si>
+    <t>Bugs?</t>
+  </si>
+  <si>
+    <t>Energy so +100</t>
   </si>
 </sst>
 </file>
@@ -738,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -851,6 +885,66 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -863,66 +957,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1389,12 +1428,267 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBD1C3D-5A83-4A9D-8EE5-5F7EF17A549A}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="21.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21.75" customHeight="1">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21.75" customHeight="1">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="G2" s="62">
+        <v>100</v>
+      </c>
+      <c r="H2" s="62">
+        <v>500</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21.75" customHeight="1">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>20000</v>
+      </c>
+      <c r="F3" s="63">
+        <v>10000</v>
+      </c>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>20000</v>
+      </c>
+      <c r="F4" s="63">
+        <v>10000</v>
+      </c>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>300</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+      <c r="E5">
+        <v>9000</v>
+      </c>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21.75" customHeight="1">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="64">
+        <v>200</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6">
+        <v>1000</v>
+      </c>
+      <c r="E6">
+        <v>9000</v>
+      </c>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21.75" customHeight="1">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>1000</v>
+      </c>
+      <c r="E7">
+        <v>20000</v>
+      </c>
+      <c r="F7" s="63">
+        <v>10000</v>
+      </c>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="21.75" customHeight="1">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8">
+        <v>200</v>
+      </c>
+      <c r="D8">
+        <v>1500</v>
+      </c>
+      <c r="E8">
+        <v>15000</v>
+      </c>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="21.75" customHeight="1">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>1500</v>
+      </c>
+      <c r="E9">
+        <v>15000</v>
+      </c>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="21.75" customHeight="1">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10">
+        <v>400</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>1000</v>
+      </c>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21.75" customHeight="1">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="64">
+        <v>500</v>
+      </c>
+      <c r="C11" s="64" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+      <c r="E11">
+        <v>1000</v>
+      </c>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G2:G11"/>
+    <mergeCell ref="H2:H11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.25" customHeight="1"/>
@@ -2386,10 +2680,10 @@
       </c>
     </row>
     <row r="12" spans="1:27" ht="29.25" customHeight="1">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="38" t="s">
         <v>130</v>
       </c>
       <c r="C12" s="27">
@@ -2562,7 +2856,7 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="29.25" customHeight="1">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="39" t="s">
         <v>82</v>
       </c>
       <c r="B14" s="27" t="s">
@@ -2738,10 +3032,10 @@
       </c>
     </row>
     <row r="16" spans="1:27" ht="29.25" customHeight="1">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="38" t="s">
         <v>130</v>
       </c>
       <c r="C16" s="27">
@@ -3006,7 +3300,7 @@
       </c>
     </row>
     <row r="19" spans="1:27" ht="29.25" customHeight="1">
-      <c r="A19" s="61" t="s">
+      <c r="A19" s="39" t="s">
         <v>91</v>
       </c>
       <c r="B19" s="27" t="s">
@@ -3094,7 +3388,7 @@
       </c>
     </row>
     <row r="20" spans="1:27" ht="29.25" customHeight="1">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="39" t="s">
         <v>105</v>
       </c>
       <c r="B20" s="27" t="s">
@@ -3182,10 +3476,10 @@
       </c>
     </row>
     <row r="21" spans="1:27" ht="29.25" customHeight="1">
-      <c r="A21" s="60" t="s">
+      <c r="A21" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="38" t="s">
         <v>130</v>
       </c>
       <c r="C21" s="27">
@@ -3272,7 +3566,7 @@
       </c>
     </row>
     <row r="22" spans="1:27" ht="29.25" customHeight="1">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="39" t="s">
         <v>70</v>
       </c>
       <c r="B22" s="27" t="s">
@@ -3939,11 +4233,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
@@ -3961,68 +4255,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="135.75" customHeight="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
     </row>
     <row r="2" spans="1:18" ht="28.35" customHeight="1">
-      <c r="A2" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
+      <c r="A2" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
     </row>
     <row r="3" spans="1:18" ht="15.95" customHeight="1">
-      <c r="C3" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39" t="s">
+      <c r="C3" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39" t="s">
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="40"/>
-      <c r="O3" s="41" t="s">
+      <c r="N3" s="60"/>
+      <c r="O3" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="41"/>
+      <c r="P3" s="61"/>
     </row>
     <row r="4" spans="1:18" s="4" customFormat="1" ht="12.4" customHeight="1">
       <c r="B4" s="4" t="s">
@@ -4055,7 +4349,7 @@
       <c r="K4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="39"/>
+      <c r="L4" s="59"/>
       <c r="M4" s="5" t="s">
         <v>11</v>
       </c>
@@ -4070,13 +4364,13 @@
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="43" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="54" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="44" t="s">
@@ -4085,70 +4379,70 @@
       <c r="E5" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="42">
+      <c r="F5" s="45">
         <v>5</v>
       </c>
-      <c r="G5" s="42">
-        <v>1</v>
-      </c>
-      <c r="H5" s="42">
+      <c r="G5" s="45">
+        <v>1</v>
+      </c>
+      <c r="H5" s="45">
         <v>0.1</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="45">
         <v>0.9</v>
       </c>
-      <c r="K5" s="42">
+      <c r="K5" s="45">
         <f t="shared" ref="K5:K6" si="0">F5*J5</f>
         <v>4.5</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="42" t="s">
+      <c r="M5" s="55"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="P5" s="42" t="s">
+      <c r="P5" s="45" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A6" s="49"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="43"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="44" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="44"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42">
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="42" t="s">
+      <c r="M6" s="55"/>
+      <c r="N6" s="55"/>
+      <c r="O6" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="P6" s="42" t="s">
+      <c r="P6" s="45" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A7" s="49"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="7" t="s">
         <v>25</v>
       </c>
@@ -4184,11 +4478,11 @@
       <c r="N7" s="9"/>
     </row>
     <row r="8" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A8" s="49"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="54" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="44" t="s">
@@ -4197,73 +4491,73 @@
       <c r="E8" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="42">
+      <c r="F8" s="45">
         <v>5</v>
       </c>
-      <c r="G8" s="42">
-        <v>1</v>
-      </c>
-      <c r="H8" s="42">
+      <c r="G8" s="45">
+        <v>1</v>
+      </c>
+      <c r="H8" s="45">
         <v>0.05</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="I8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="42">
+      <c r="J8" s="45">
         <v>0.7</v>
       </c>
-      <c r="K8" s="42">
+      <c r="K8" s="45">
         <f>F8*J8</f>
         <v>3.5</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="42"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="45"/>
     </row>
     <row r="9" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A9" s="49"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="43"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="44" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="44"/>
-      <c r="F9" s="42">
+      <c r="F9" s="45">
         <v>5</v>
       </c>
-      <c r="G9" s="42">
-        <v>1</v>
-      </c>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42" t="s">
+      <c r="G9" s="45">
+        <v>1</v>
+      </c>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
       <c r="L9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="45"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="42"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="45"/>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="45"/>
     </row>
     <row r="10" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A10" s="49"/>
-      <c r="B10" s="43" t="s">
+      <c r="A10" s="43"/>
+      <c r="B10" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="54" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -4311,11 +4605,11 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A11" s="49"/>
-      <c r="B11" s="43" t="s">
+      <c r="A11" s="43"/>
+      <c r="B11" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="54" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -4363,11 +4657,11 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A12" s="49"/>
-      <c r="B12" s="43" t="s">
+      <c r="A12" s="43"/>
+      <c r="B12" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="54" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -4415,11 +4709,11 @@
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A13" s="49"/>
-      <c r="B13" s="43" t="s">
+      <c r="A13" s="43"/>
+      <c r="B13" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="54" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -4467,11 +4761,11 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A14" s="49"/>
-      <c r="B14" s="43" t="s">
+      <c r="A14" s="43"/>
+      <c r="B14" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="54" t="s">
         <v>41</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -4519,11 +4813,11 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A15" s="49"/>
-      <c r="B15" s="43" t="s">
+      <c r="A15" s="43"/>
+      <c r="B15" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="54" t="s">
         <v>43</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -4571,11 +4865,11 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A16" s="49"/>
-      <c r="B16" s="43" t="s">
+      <c r="A16" s="43"/>
+      <c r="B16" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="54" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -4623,11 +4917,11 @@
       </c>
     </row>
     <row r="17" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A17" s="49"/>
-      <c r="B17" s="43" t="s">
+      <c r="A17" s="43"/>
+      <c r="B17" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="54" t="s">
         <v>47</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -4675,11 +4969,11 @@
       </c>
     </row>
     <row r="18" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A18" s="49"/>
-      <c r="B18" s="43" t="s">
+      <c r="A18" s="43"/>
+      <c r="B18" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="54" t="s">
         <v>49</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -4713,7 +5007,7 @@
       <c r="Q18" s="10"/>
     </row>
     <row r="19" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="57" t="s">
         <v>51</v>
       </c>
       <c r="B19" s="14" t="s">
@@ -4766,11 +5060,11 @@
       </c>
     </row>
     <row r="20" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A20" s="46"/>
-      <c r="B20" s="47" t="s">
+      <c r="A20" s="57"/>
+      <c r="B20" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="42" t="s">
         <v>53</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -4779,13 +5073,13 @@
       <c r="E20" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="42">
+      <c r="F20" s="45">
         <v>3</v>
       </c>
-      <c r="G20" s="42">
-        <v>1</v>
-      </c>
-      <c r="H20" s="42">
+      <c r="G20" s="45">
+        <v>1</v>
+      </c>
+      <c r="H20" s="45">
         <v>0.08</v>
       </c>
       <c r="I20" s="12" t="s">
@@ -4798,7 +5092,7 @@
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="L20" s="50"/>
+      <c r="L20" s="47"/>
       <c r="M20" s="16">
         <f>J20/J5</f>
         <v>0.27777777777777779</v>
@@ -4817,16 +5111,16 @@
       </c>
     </row>
     <row r="21" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A21" s="46"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="2" t="s">
         <v>55</v>
       </c>
       <c r="E21" s="44"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
       <c r="I21" s="12" t="s">
         <v>56</v>
       </c>
@@ -4837,7 +5131,7 @@
         <f>F20*J21</f>
         <v>1.5</v>
       </c>
-      <c r="L21" s="50"/>
+      <c r="L21" s="47"/>
       <c r="M21" s="16">
         <f>J21/J18</f>
         <v>0.5</v>
@@ -4849,11 +5143,11 @@
       <c r="O21" s="10"/>
     </row>
     <row r="22" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A22" s="46"/>
-      <c r="B22" s="47" t="s">
+      <c r="A22" s="57"/>
+      <c r="B22" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="42" t="s">
         <v>57</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -4862,13 +5156,13 @@
       <c r="E22" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="42">
+      <c r="F22" s="45">
         <v>2.5</v>
       </c>
-      <c r="G22" s="42">
-        <v>1</v>
-      </c>
-      <c r="H22" s="42">
+      <c r="G22" s="45">
+        <v>1</v>
+      </c>
+      <c r="H22" s="45">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -4881,7 +5175,7 @@
         <f>F22*J22</f>
         <v>0.875</v>
       </c>
-      <c r="L22" s="50" t="s">
+      <c r="L22" s="47" t="s">
         <v>58</v>
       </c>
       <c r="M22" s="16">
@@ -4895,16 +5189,16 @@
       <c r="O22" s="10"/>
     </row>
     <row r="23" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A23" s="46"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
       <c r="D23" s="2" t="s">
         <v>55</v>
       </c>
       <c r="E23" s="44"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
       <c r="I23" s="13" t="s">
         <v>56</v>
       </c>
@@ -4915,7 +5209,7 @@
         <f>F22*J23</f>
         <v>0.625</v>
       </c>
-      <c r="L23" s="50"/>
+      <c r="L23" s="47"/>
       <c r="M23" s="16">
         <f>J23/J18</f>
         <v>0.25</v>
@@ -4927,7 +5221,7 @@
       <c r="O23" s="10"/>
     </row>
     <row r="24" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A24" s="46"/>
+      <c r="A24" s="57"/>
       <c r="B24" s="14" t="s">
         <v>31</v>
       </c>
@@ -4973,26 +5267,26 @@
       <c r="O24" s="10"/>
     </row>
     <row r="25" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="47"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="44" t="s">
         <v>63</v>
       </c>
       <c r="E25" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="F25" s="42">
+      <c r="F25" s="45">
         <v>5</v>
       </c>
-      <c r="G25" s="42">
-        <v>1</v>
-      </c>
-      <c r="H25" s="42">
+      <c r="G25" s="45">
+        <v>1</v>
+      </c>
+      <c r="H25" s="45">
         <v>0.32</v>
       </c>
       <c r="I25" s="15" t="s">
@@ -5005,7 +5299,7 @@
         <f t="shared" si="3"/>
         <v>1.75</v>
       </c>
-      <c r="L25" s="50"/>
+      <c r="L25" s="47"/>
       <c r="M25" s="16">
         <f>J25/J8</f>
         <v>0.5</v>
@@ -5014,20 +5308,20 @@
         <f>K25/K8</f>
         <v>0.5</v>
       </c>
-      <c r="O25" s="54">
+      <c r="O25" s="40">
         <f>SUM(N25:N26)</f>
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A26" s="49"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
       <c r="D26" s="44"/>
       <c r="E26" s="44"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
       <c r="I26" s="1" t="s">
         <v>39</v>
       </c>
@@ -5038,7 +5332,7 @@
         <f>F25*J26</f>
         <v>1.75</v>
       </c>
-      <c r="L26" s="50"/>
+      <c r="L26" s="47"/>
       <c r="M26" s="16">
         <f>J26/J13</f>
         <v>0.5</v>
@@ -5047,14 +5341,14 @@
         <f>K26/K13</f>
         <v>0.5</v>
       </c>
-      <c r="O26" s="54"/>
+      <c r="O26" s="40"/>
     </row>
     <row r="27" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A27" s="49"/>
-      <c r="B27" s="47" t="s">
+      <c r="A27" s="43"/>
+      <c r="B27" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="47"/>
+      <c r="C27" s="42"/>
       <c r="D27" s="2" t="s">
         <v>66</v>
       </c>
@@ -5095,11 +5389,11 @@
       </c>
     </row>
     <row r="28" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A28" s="49"/>
-      <c r="B28" s="47" t="s">
+      <c r="A28" s="43"/>
+      <c r="B28" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="47"/>
+      <c r="C28" s="42"/>
       <c r="D28" s="2" t="s">
         <v>19</v>
       </c>
@@ -5142,11 +5436,11 @@
       </c>
     </row>
     <row r="29" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A29" s="49"/>
-      <c r="B29" s="47" t="s">
+      <c r="A29" s="43"/>
+      <c r="B29" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="47"/>
+      <c r="C29" s="42"/>
       <c r="D29" s="2" t="s">
         <v>71</v>
       </c>
@@ -5187,11 +5481,11 @@
       </c>
     </row>
     <row r="30" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A30" s="49"/>
-      <c r="B30" s="47" t="s">
+      <c r="A30" s="43"/>
+      <c r="B30" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="47"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="2" t="s">
         <v>73</v>
       </c>
@@ -5232,11 +5526,11 @@
       </c>
     </row>
     <row r="31" spans="1:18" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A31" s="49"/>
-      <c r="B31" s="47" t="s">
+      <c r="A31" s="43"/>
+      <c r="B31" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="47"/>
+      <c r="C31" s="42"/>
       <c r="D31" s="19" t="s">
         <v>75</v>
       </c>
@@ -5279,24 +5573,24 @@
       </c>
     </row>
     <row r="32" spans="1:18" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A32" s="49"/>
-      <c r="B32" s="47" t="s">
+      <c r="A32" s="43"/>
+      <c r="B32" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="47"/>
-      <c r="D32" s="51" t="s">
+      <c r="C32" s="42"/>
+      <c r="D32" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="51" t="s">
+      <c r="E32" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="F32" s="52">
+      <c r="F32" s="50">
         <v>3.5</v>
       </c>
-      <c r="G32" s="52">
-        <v>1</v>
-      </c>
-      <c r="H32" s="52">
+      <c r="G32" s="50">
+        <v>1</v>
+      </c>
+      <c r="H32" s="50">
         <v>3.1</v>
       </c>
       <c r="I32" s="17" t="s">
@@ -5309,7 +5603,7 @@
         <f t="shared" si="4"/>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="L32" s="53" t="s">
+      <c r="L32" s="48" t="s">
         <v>79</v>
       </c>
       <c r="M32" s="21">
@@ -5320,20 +5614,20 @@
         <f t="shared" si="7"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="O32" s="54">
+      <c r="O32" s="40">
         <f>SUM(N32:N33)</f>
         <v>1.1115555555555556</v>
       </c>
     </row>
     <row r="33" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A33" s="49"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="52"/>
-      <c r="H33" s="52"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50"/>
       <c r="I33" s="17" t="s">
         <v>56</v>
       </c>
@@ -5344,7 +5638,7 @@
         <f>F32*J33</f>
         <v>2.0020000000000002</v>
       </c>
-      <c r="L33" s="53"/>
+      <c r="L33" s="48"/>
       <c r="M33" s="21">
         <f t="shared" si="6"/>
         <v>0.57200000000000006</v>
@@ -5353,27 +5647,27 @@
         <f t="shared" si="7"/>
         <v>0.44488888888888894</v>
       </c>
-      <c r="O33" s="54"/>
+      <c r="O33" s="40"/>
     </row>
     <row r="34" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A34" s="49"/>
-      <c r="B34" s="47" t="s">
+      <c r="A34" s="43"/>
+      <c r="B34" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="47"/>
-      <c r="D34" s="51" t="s">
+      <c r="C34" s="42"/>
+      <c r="D34" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="51" t="s">
+      <c r="E34" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="F34" s="52">
+      <c r="F34" s="50">
         <v>5</v>
       </c>
-      <c r="G34" s="52">
-        <v>1</v>
-      </c>
-      <c r="H34" s="52">
+      <c r="G34" s="50">
+        <v>1</v>
+      </c>
+      <c r="H34" s="50">
         <v>1.3</v>
       </c>
       <c r="I34" s="17" t="s">
@@ -5386,7 +5680,7 @@
         <f>F34*J34</f>
         <v>1.1700000000000002</v>
       </c>
-      <c r="L34" s="53"/>
+      <c r="L34" s="48"/>
       <c r="M34" s="21">
         <f>J34/J8</f>
         <v>0.33428571428571435</v>
@@ -5395,20 +5689,20 @@
         <f>K34/K8</f>
         <v>0.33428571428571435</v>
       </c>
-      <c r="O34" s="54">
+      <c r="O34" s="40">
         <f>SUM(N34:N35)</f>
         <v>1.0009523809523808</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A35" s="49"/>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
       <c r="I35" s="17" t="s">
         <v>35</v>
       </c>
@@ -5419,7 +5713,7 @@
         <f>F34*J35</f>
         <v>1</v>
       </c>
-      <c r="L35" s="53"/>
+      <c r="L35" s="48"/>
       <c r="M35" s="21">
         <f>J35/J11</f>
         <v>0.66666666666666663</v>
@@ -5428,27 +5722,27 @@
         <f>K35/K11</f>
         <v>0.66666666666666652</v>
       </c>
-      <c r="O35" s="54"/>
+      <c r="O35" s="40"/>
     </row>
     <row r="36" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A36" s="49"/>
-      <c r="B36" s="47" t="s">
+      <c r="A36" s="43"/>
+      <c r="B36" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="C36" s="47"/>
-      <c r="D36" s="51" t="s">
+      <c r="C36" s="42"/>
+      <c r="D36" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="E36" s="51" t="s">
+      <c r="E36" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="F36" s="52">
+      <c r="F36" s="50">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G36" s="52">
-        <v>1</v>
-      </c>
-      <c r="H36" s="52">
+      <c r="G36" s="50">
+        <v>1</v>
+      </c>
+      <c r="H36" s="50">
         <v>0.5</v>
       </c>
       <c r="I36" s="17" t="s">
@@ -5461,7 +5755,7 @@
         <f>F36*J36</f>
         <v>2.5299999999999998</v>
       </c>
-      <c r="L36" s="53"/>
+      <c r="L36" s="48"/>
       <c r="M36" s="21">
         <f>J36/J13</f>
         <v>0.78571428571428581</v>
@@ -5470,20 +5764,20 @@
         <f>K36/K13</f>
         <v>0.72285714285714275</v>
       </c>
-      <c r="O36" s="54">
+      <c r="O36" s="40">
         <f>SUM(N36:N37)</f>
         <v>0.94774603174603167</v>
       </c>
     </row>
     <row r="37" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A37" s="49"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
+      <c r="A37" s="43"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
       <c r="I37" s="17" t="s">
         <v>56</v>
       </c>
@@ -5494,7 +5788,7 @@
         <f>F36*J37</f>
         <v>1.012</v>
       </c>
-      <c r="L37" s="53"/>
+      <c r="L37" s="48"/>
       <c r="M37" s="21">
         <f>J37/J18</f>
         <v>0.22</v>
@@ -5503,27 +5797,27 @@
         <f>K37/K18</f>
         <v>0.22488888888888889</v>
       </c>
-      <c r="O37" s="54"/>
+      <c r="O37" s="40"/>
     </row>
     <row r="38" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A38" s="49"/>
-      <c r="B38" s="47" t="s">
+      <c r="A38" s="43"/>
+      <c r="B38" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="47"/>
-      <c r="D38" s="51" t="s">
+      <c r="C38" s="42"/>
+      <c r="D38" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="E38" s="51" t="s">
+      <c r="E38" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="52">
+      <c r="F38" s="50">
         <v>5.2</v>
       </c>
-      <c r="G38" s="52">
-        <v>1</v>
-      </c>
-      <c r="H38" s="52">
+      <c r="G38" s="50">
+        <v>1</v>
+      </c>
+      <c r="H38" s="50">
         <v>0.25</v>
       </c>
       <c r="I38" s="17" t="s">
@@ -5536,7 +5830,7 @@
         <f>F38*J38</f>
         <v>2.8600000000000003</v>
       </c>
-      <c r="L38" s="55"/>
+      <c r="L38" s="52"/>
       <c r="M38" s="21">
         <f>J38/J8</f>
         <v>0.78571428571428581</v>
@@ -5545,20 +5839,20 @@
         <f>K38/K8</f>
         <v>0.81714285714285728</v>
       </c>
-      <c r="O38" s="54">
+      <c r="O38" s="40">
         <f>SUM(N38:N39)</f>
         <v>1.1142857142857143</v>
       </c>
     </row>
     <row r="39" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A39" s="49"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="47"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
+      <c r="A39" s="43"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="50"/>
       <c r="I39" s="17" t="s">
         <v>43</v>
       </c>
@@ -5569,7 +5863,7 @@
         <f>F38*J39</f>
         <v>1.0400000000000001E-2</v>
       </c>
-      <c r="L39" s="55"/>
+      <c r="L39" s="52"/>
       <c r="M39" s="21">
         <f>J39/J15</f>
         <v>0.2</v>
@@ -5578,27 +5872,27 @@
         <f>K39/K15</f>
         <v>0.29714285714285715</v>
       </c>
-      <c r="O39" s="54"/>
+      <c r="O39" s="40"/>
     </row>
     <row r="40" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A40" s="49"/>
-      <c r="B40" s="47" t="s">
+      <c r="A40" s="43"/>
+      <c r="B40" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="47"/>
-      <c r="D40" s="56" t="s">
+      <c r="C40" s="42"/>
+      <c r="D40" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="E40" s="56" t="s">
+      <c r="E40" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="52">
+      <c r="F40" s="50">
         <v>4.2</v>
       </c>
-      <c r="G40" s="52">
-        <v>1</v>
-      </c>
-      <c r="H40" s="52">
+      <c r="G40" s="50">
+        <v>1</v>
+      </c>
+      <c r="H40" s="50">
         <v>1.9</v>
       </c>
       <c r="I40" s="17" t="s">
@@ -5611,7 +5905,7 @@
         <f>F40*J40</f>
         <v>0.504</v>
       </c>
-      <c r="L40" s="53" t="s">
+      <c r="L40" s="48" t="s">
         <v>88</v>
       </c>
       <c r="M40" s="21">
@@ -5622,20 +5916,20 @@
         <f>K40/K13</f>
         <v>0.14399999999999999</v>
       </c>
-      <c r="O40" s="54">
+      <c r="O40" s="40">
         <f>SUM(N40:N42)</f>
         <v>1.0226666666666666</v>
       </c>
     </row>
     <row r="41" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A41" s="49"/>
-      <c r="B41" s="49"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="52"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="52"/>
+      <c r="A41" s="43"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50"/>
       <c r="I41" s="17" t="s">
         <v>37</v>
       </c>
@@ -5646,7 +5940,7 @@
         <f>F40*J41</f>
         <v>2.52E-2</v>
       </c>
-      <c r="L41" s="53"/>
+      <c r="L41" s="48"/>
       <c r="M41" s="21">
         <f>J41/J12</f>
         <v>0.8571428571428571</v>
@@ -5655,17 +5949,17 @@
         <f>K41/K12</f>
         <v>0.72</v>
       </c>
-      <c r="O41" s="54"/>
+      <c r="O41" s="40"/>
     </row>
     <row r="42" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A42" s="49"/>
-      <c r="B42" s="49"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="52"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
       <c r="I42" s="17" t="s">
         <v>56</v>
       </c>
@@ -5676,7 +5970,7 @@
         <f>F40*J42</f>
         <v>0.71400000000000008</v>
       </c>
-      <c r="L42" s="53"/>
+      <c r="L42" s="48"/>
       <c r="M42" s="21">
         <f>J42/J18</f>
         <v>0.17</v>
@@ -5685,27 +5979,27 @@
         <f>K42/K18</f>
         <v>0.15866666666666668</v>
       </c>
-      <c r="O42" s="54"/>
+      <c r="O42" s="40"/>
     </row>
     <row r="43" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A43" s="49"/>
-      <c r="B43" s="47" t="s">
+      <c r="A43" s="43"/>
+      <c r="B43" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="47"/>
-      <c r="D43" s="51" t="s">
+      <c r="C43" s="42"/>
+      <c r="D43" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="E43" s="51" t="s">
+      <c r="E43" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="F43" s="57">
+      <c r="F43" s="51">
         <v>1.9</v>
       </c>
-      <c r="G43" s="52">
-        <v>1</v>
-      </c>
-      <c r="H43" s="52">
+      <c r="G43" s="50">
+        <v>1</v>
+      </c>
+      <c r="H43" s="50">
         <v>3.2</v>
       </c>
       <c r="I43" s="17" t="s">
@@ -5718,7 +6012,7 @@
         <f>F43*J43</f>
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="L43" s="53"/>
+      <c r="L43" s="48"/>
       <c r="M43" s="21">
         <f>J43/J16</f>
         <v>0.6</v>
@@ -5727,20 +6021,20 @@
         <f>K43/K16</f>
         <v>0.71250000000000002</v>
       </c>
-      <c r="O43" s="54">
+      <c r="O43" s="40">
         <f>SUM(N43:N44)</f>
         <v>1.0545</v>
       </c>
     </row>
     <row r="44" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A44" s="49"/>
-      <c r="B44" s="49"/>
-      <c r="C44" s="47"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
+      <c r="A44" s="43"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
       <c r="I44" s="17" t="s">
         <v>33</v>
       </c>
@@ -5751,7 +6045,7 @@
         <f>F43*J44</f>
         <v>0.68399999999999994</v>
       </c>
-      <c r="L44" s="53"/>
+      <c r="L44" s="48"/>
       <c r="M44" s="21">
         <f>J44/J10</f>
         <v>0.89999999999999991</v>
@@ -5760,27 +6054,27 @@
         <f>K44/K10</f>
         <v>0.34199999999999997</v>
       </c>
-      <c r="O44" s="54"/>
+      <c r="O44" s="40"/>
     </row>
     <row r="45" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A45" s="49"/>
-      <c r="B45" s="47" t="s">
+      <c r="A45" s="43"/>
+      <c r="B45" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="47"/>
-      <c r="D45" s="51" t="s">
+      <c r="C45" s="42"/>
+      <c r="D45" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="E45" s="51" t="s">
+      <c r="E45" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="F45" s="42">
+      <c r="F45" s="45">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G45" s="42">
-        <v>1</v>
-      </c>
-      <c r="H45" s="52">
+      <c r="G45" s="45">
+        <v>1</v>
+      </c>
+      <c r="H45" s="50">
         <v>0.5</v>
       </c>
       <c r="I45" s="17" t="s">
@@ -5793,7 +6087,7 @@
         <f>F45*J45</f>
         <v>1.8039999999999998</v>
       </c>
-      <c r="L45" s="53"/>
+      <c r="L45" s="48"/>
       <c r="M45" s="21">
         <f>J45/J13</f>
         <v>0.62857142857142867</v>
@@ -5802,20 +6096,20 @@
         <f>K45/K13</f>
         <v>0.51542857142857135</v>
       </c>
-      <c r="O45" s="54">
+      <c r="O45" s="40">
         <f>SUM(N45:N46)</f>
         <v>1.0256507936507935</v>
       </c>
     </row>
     <row r="46" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
-      <c r="C46" s="47"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45"/>
       <c r="I46" s="17" t="s">
         <v>56</v>
       </c>
@@ -5826,7 +6120,7 @@
         <f>F45*J46</f>
         <v>2.2959999999999998</v>
       </c>
-      <c r="L46" s="53"/>
+      <c r="L46" s="48"/>
       <c r="M46" s="21">
         <f>J46/J18</f>
         <v>0.56000000000000005</v>
@@ -5835,14 +6129,14 @@
         <f>K46/K18</f>
         <v>0.51022222222222213</v>
       </c>
-      <c r="O46" s="54"/>
+      <c r="O46" s="40"/>
     </row>
     <row r="47" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A47" s="49"/>
-      <c r="B47" s="47" t="s">
+      <c r="A47" s="43"/>
+      <c r="B47" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="C47" s="47"/>
+      <c r="C47" s="42"/>
       <c r="D47" s="19" t="s">
         <v>94</v>
       </c>
@@ -5885,11 +6179,11 @@
       </c>
     </row>
     <row r="48" spans="1:15" s="17" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A48" s="49"/>
-      <c r="B48" s="47" t="s">
+      <c r="A48" s="43"/>
+      <c r="B48" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="47"/>
+      <c r="C48" s="42"/>
       <c r="D48" s="19" t="s">
         <v>97</v>
       </c>
@@ -5932,24 +6226,24 @@
       </c>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A49" s="49"/>
-      <c r="B49" s="47" t="s">
+      <c r="A49" s="43"/>
+      <c r="B49" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="C49" s="47"/>
+      <c r="C49" s="42"/>
       <c r="D49" s="44" t="s">
         <v>100</v>
       </c>
       <c r="E49" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="F49" s="42">
+      <c r="F49" s="45">
         <v>1.8</v>
       </c>
-      <c r="G49" s="42">
-        <v>1</v>
-      </c>
-      <c r="H49" s="42">
+      <c r="G49" s="45">
+        <v>1</v>
+      </c>
+      <c r="H49" s="45">
         <v>0.7</v>
       </c>
       <c r="I49" s="1" t="s">
@@ -5962,7 +6256,7 @@
         <f t="shared" si="8"/>
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="L49" s="50"/>
+      <c r="L49" s="47"/>
       <c r="M49" s="16">
         <f t="shared" ref="M49:M52" si="10">J49/J14</f>
         <v>0.44999999999999996</v>
@@ -5971,20 +6265,20 @@
         <f t="shared" ref="N49:N52" si="11">K49/K14</f>
         <v>0.53999999999999992</v>
       </c>
-      <c r="O49" s="54">
+      <c r="O49" s="40">
         <f>SUM(N49:N50)</f>
         <v>1.0028571428571429</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A50" s="49"/>
-      <c r="B50" s="49"/>
-      <c r="C50" s="47"/>
+      <c r="A50" s="43"/>
+      <c r="B50" s="43"/>
+      <c r="C50" s="42"/>
       <c r="D50" s="44"/>
       <c r="E50" s="44"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
       <c r="I50" s="1" t="s">
         <v>43</v>
       </c>
@@ -5995,7 +6289,7 @@
         <f>F49*J50</f>
         <v>1.6200000000000003E-2</v>
       </c>
-      <c r="L50" s="50"/>
+      <c r="L50" s="47"/>
       <c r="M50" s="16">
         <f t="shared" si="10"/>
         <v>0.90000000000000013</v>
@@ -6004,14 +6298,14 @@
         <f t="shared" si="11"/>
         <v>0.46285714285714291</v>
       </c>
-      <c r="O50" s="54"/>
+      <c r="O50" s="40"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A51" s="49"/>
-      <c r="B51" s="47" t="s">
+      <c r="A51" s="43"/>
+      <c r="B51" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="C51" s="47"/>
+      <c r="C51" s="42"/>
       <c r="D51" s="2" t="s">
         <v>102</v>
       </c>
@@ -6052,11 +6346,11 @@
       </c>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A52" s="49"/>
-      <c r="B52" s="47" t="s">
+      <c r="A52" s="43"/>
+      <c r="B52" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="47"/>
+      <c r="C52" s="42"/>
       <c r="D52" s="2" t="s">
         <v>104</v>
       </c>
@@ -6097,24 +6391,24 @@
       </c>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A53" s="49"/>
-      <c r="B53" s="47" t="s">
+      <c r="A53" s="43"/>
+      <c r="B53" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="C53" s="47"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="44" t="s">
         <v>106</v>
       </c>
       <c r="E53" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="F53" s="42">
+      <c r="F53" s="45">
         <v>8.8000000000000007</v>
       </c>
-      <c r="G53" s="42">
-        <v>1</v>
-      </c>
-      <c r="H53" s="42">
+      <c r="G53" s="45">
+        <v>1</v>
+      </c>
+      <c r="H53" s="45">
         <v>0.35</v>
       </c>
       <c r="I53" s="1" t="s">
@@ -6127,7 +6421,7 @@
         <f t="shared" si="12"/>
         <v>1.7600000000000002</v>
       </c>
-      <c r="L53" s="50" t="s">
+      <c r="L53" s="47" t="s">
         <v>88</v>
       </c>
       <c r="M53" s="16">
@@ -6138,20 +6432,20 @@
         <f>K53/K13</f>
         <v>0.50285714285714289</v>
       </c>
-      <c r="O53" s="54">
+      <c r="O53" s="40">
         <f>SUM(N53:N54)</f>
         <v>1.0057142857142858</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A54" s="49"/>
-      <c r="B54" s="49"/>
-      <c r="C54" s="47"/>
+      <c r="A54" s="43"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="42"/>
       <c r="D54" s="44"/>
       <c r="E54" s="44"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="45"/>
+      <c r="H54" s="45"/>
       <c r="I54" s="1" t="s">
         <v>37</v>
       </c>
@@ -6162,7 +6456,7 @@
         <f>F53*J54</f>
         <v>1.7600000000000001E-2</v>
       </c>
-      <c r="L54" s="50"/>
+      <c r="L54" s="47"/>
       <c r="M54" s="16">
         <f t="shared" ref="M54:M55" si="14">J54/J12</f>
         <v>0.2857142857142857</v>
@@ -6171,27 +6465,27 @@
         <f t="shared" ref="N54:N55" si="15">K54/K12</f>
         <v>0.50285714285714289</v>
       </c>
-      <c r="O54" s="54"/>
+      <c r="O54" s="40"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A55" s="49"/>
-      <c r="B55" s="47" t="s">
+      <c r="A55" s="43"/>
+      <c r="B55" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="47"/>
+      <c r="C55" s="42"/>
       <c r="D55" s="44" t="s">
         <v>108</v>
       </c>
       <c r="E55" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="F55" s="42">
+      <c r="F55" s="45">
         <v>6.3</v>
       </c>
-      <c r="G55" s="42">
-        <v>1</v>
-      </c>
-      <c r="H55" s="42">
+      <c r="G55" s="45">
+        <v>1</v>
+      </c>
+      <c r="H55" s="45">
         <v>0.55000000000000004</v>
       </c>
       <c r="I55" s="1" t="s">
@@ -6204,7 +6498,7 @@
         <f>F55*J55</f>
         <v>1.89</v>
       </c>
-      <c r="L55" s="50"/>
+      <c r="L55" s="47"/>
       <c r="M55" s="16">
         <f t="shared" si="14"/>
         <v>0.4285714285714286</v>
@@ -6213,20 +6507,20 @@
         <f t="shared" si="15"/>
         <v>0.53999999999999992</v>
       </c>
-      <c r="O55" s="54">
+      <c r="O55" s="40">
         <f>SUM(N55:N56)</f>
         <v>1.0799999999999998</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A56" s="49"/>
-      <c r="B56" s="49"/>
-      <c r="C56" s="47"/>
+      <c r="A56" s="43"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="42"/>
       <c r="D56" s="44"/>
       <c r="E56" s="44"/>
-      <c r="F56" s="42"/>
-      <c r="G56" s="42"/>
-      <c r="H56" s="42"/>
+      <c r="F56" s="45"/>
+      <c r="G56" s="45"/>
+      <c r="H56" s="45"/>
       <c r="I56" s="1" t="s">
         <v>37</v>
       </c>
@@ -6237,7 +6531,7 @@
         <f>F55*J56</f>
         <v>1.89E-2</v>
       </c>
-      <c r="L56" s="50"/>
+      <c r="L56" s="47"/>
       <c r="M56" s="16">
         <f>J56/J12</f>
         <v>0.42857142857142855</v>
@@ -6246,27 +6540,27 @@
         <f>K56/K12</f>
         <v>0.53999999999999992</v>
       </c>
-      <c r="O56" s="54"/>
+      <c r="O56" s="40"/>
     </row>
     <row r="57" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A57" s="49"/>
-      <c r="B57" s="47" t="s">
+      <c r="A57" s="43"/>
+      <c r="B57" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="C57" s="47"/>
+      <c r="C57" s="42"/>
       <c r="D57" s="44" t="s">
         <v>110</v>
       </c>
       <c r="E57" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="F57" s="42">
+      <c r="F57" s="45">
         <v>5</v>
       </c>
-      <c r="G57" s="42">
-        <v>1</v>
-      </c>
-      <c r="H57" s="42">
+      <c r="G57" s="45">
+        <v>1</v>
+      </c>
+      <c r="H57" s="45">
         <v>1.0249999999999999</v>
       </c>
       <c r="I57" s="1" t="s">
@@ -6279,7 +6573,7 @@
         <f>F57*J57</f>
         <v>1.75</v>
       </c>
-      <c r="L57" s="50"/>
+      <c r="L57" s="47"/>
       <c r="M57" s="16">
         <f>J57/J8</f>
         <v>0.5</v>
@@ -6288,20 +6582,20 @@
         <f>K57/K8</f>
         <v>0.5</v>
       </c>
-      <c r="O57" s="54">
+      <c r="O57" s="40">
         <f>SUM(N57:N58)</f>
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A58" s="49"/>
-      <c r="B58" s="49"/>
-      <c r="C58" s="47"/>
+      <c r="A58" s="43"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="42"/>
       <c r="D58" s="44"/>
       <c r="E58" s="44"/>
-      <c r="F58" s="42"/>
-      <c r="G58" s="42"/>
-      <c r="H58" s="42"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="45"/>
       <c r="I58" s="1" t="s">
         <v>33</v>
       </c>
@@ -6312,7 +6606,7 @@
         <f>F57*J58</f>
         <v>1</v>
       </c>
-      <c r="L58" s="50"/>
+      <c r="L58" s="47"/>
       <c r="M58" s="16">
         <f>J58/J10</f>
         <v>0.5</v>
@@ -6321,27 +6615,27 @@
         <f>K58/K10</f>
         <v>0.5</v>
       </c>
-      <c r="O58" s="54"/>
+      <c r="O58" s="40"/>
     </row>
     <row r="59" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A59" s="49"/>
-      <c r="B59" s="47" t="s">
+      <c r="A59" s="43"/>
+      <c r="B59" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="C59" s="47"/>
+      <c r="C59" s="42"/>
       <c r="D59" s="44" t="s">
         <v>112</v>
       </c>
       <c r="E59" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="F59" s="42">
+      <c r="F59" s="45">
         <v>5</v>
       </c>
-      <c r="G59" s="42">
-        <v>1</v>
-      </c>
-      <c r="H59" s="42">
+      <c r="G59" s="45">
+        <v>1</v>
+      </c>
+      <c r="H59" s="45">
         <v>0.67200000000000004</v>
       </c>
       <c r="I59" s="1" t="s">
@@ -6354,7 +6648,7 @@
         <f>F59*J59</f>
         <v>1</v>
       </c>
-      <c r="L59" s="58"/>
+      <c r="L59" s="46"/>
       <c r="M59" s="16">
         <f t="shared" ref="M59:M60" si="16">J59/J10</f>
         <v>0.5</v>
@@ -6363,20 +6657,20 @@
         <f t="shared" ref="N59:N60" si="17">K59/K10</f>
         <v>0.5</v>
       </c>
-      <c r="O59" s="54">
+      <c r="O59" s="40">
         <f>SUM(N59:N60)</f>
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A60" s="49"/>
-      <c r="B60" s="47"/>
-      <c r="C60" s="47"/>
+      <c r="A60" s="43"/>
+      <c r="B60" s="42"/>
+      <c r="C60" s="42"/>
       <c r="D60" s="44"/>
       <c r="E60" s="44"/>
-      <c r="F60" s="42"/>
-      <c r="G60" s="42"/>
-      <c r="H60" s="42"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="45"/>
+      <c r="H60" s="45"/>
       <c r="I60" s="1" t="s">
         <v>35</v>
       </c>
@@ -6387,7 +6681,7 @@
         <f>F59*J60</f>
         <v>0.75</v>
       </c>
-      <c r="L60" s="58"/>
+      <c r="L60" s="46"/>
       <c r="M60" s="16">
         <f t="shared" si="16"/>
         <v>0.49999999999999989</v>
@@ -6396,27 +6690,27 @@
         <f t="shared" si="17"/>
         <v>0.49999999999999994</v>
       </c>
-      <c r="O60" s="54"/>
+      <c r="O60" s="40"/>
     </row>
     <row r="61" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A61" s="49"/>
-      <c r="B61" s="47" t="s">
+      <c r="A61" s="43"/>
+      <c r="B61" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="C61" s="47"/>
+      <c r="C61" s="42"/>
       <c r="D61" s="44" t="s">
         <v>114</v>
       </c>
       <c r="E61" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="F61" s="42">
+      <c r="F61" s="45">
         <v>5</v>
       </c>
-      <c r="G61" s="42">
-        <v>1</v>
-      </c>
-      <c r="H61" s="42">
+      <c r="G61" s="45">
+        <v>1</v>
+      </c>
+      <c r="H61" s="45">
         <v>0.67200000000000004</v>
       </c>
       <c r="I61" s="1" t="s">
@@ -6429,7 +6723,7 @@
         <f>F61*J61</f>
         <v>1.165</v>
       </c>
-      <c r="L61" s="58"/>
+      <c r="L61" s="46"/>
       <c r="M61" s="16">
         <f>J61/J8</f>
         <v>0.33285714285714291</v>
@@ -6438,20 +6732,20 @@
         <f>K61/K8</f>
         <v>0.33285714285714285</v>
       </c>
-      <c r="O61" s="54">
+      <c r="O61" s="40">
         <f>SUM(N61:N63)</f>
         <v>1.0011904761904762</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A62" s="49"/>
-      <c r="B62" s="47"/>
-      <c r="C62" s="47"/>
+      <c r="A62" s="43"/>
+      <c r="B62" s="42"/>
+      <c r="C62" s="42"/>
       <c r="D62" s="44"/>
       <c r="E62" s="44"/>
-      <c r="F62" s="42"/>
-      <c r="G62" s="42"/>
-      <c r="H62" s="42"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="45"/>
       <c r="I62" s="1" t="s">
         <v>33</v>
       </c>
@@ -6462,7 +6756,7 @@
         <f>F61*J62</f>
         <v>0.67</v>
       </c>
-      <c r="L62" s="58"/>
+      <c r="L62" s="46"/>
       <c r="M62" s="16">
         <f t="shared" ref="M62:M63" si="18">J62/J10</f>
         <v>0.33500000000000002</v>
@@ -6471,19 +6765,19 @@
         <f t="shared" ref="N62:N63" si="19">K62/K10</f>
         <v>0.33500000000000002</v>
       </c>
-      <c r="O62" s="54"/>
+      <c r="O62" s="40"/>
     </row>
     <row r="63" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A63" s="49"/>
-      <c r="B63" s="47"/>
-      <c r="C63" s="47"/>
+      <c r="A63" s="43"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="42"/>
       <c r="D63" s="44"/>
       <c r="E63" s="44"/>
-      <c r="F63" s="42"/>
-      <c r="G63" s="42">
-        <v>1</v>
-      </c>
-      <c r="H63" s="42"/>
+      <c r="F63" s="45"/>
+      <c r="G63" s="45">
+        <v>1</v>
+      </c>
+      <c r="H63" s="45"/>
       <c r="I63" s="1" t="s">
         <v>35</v>
       </c>
@@ -6494,7 +6788,7 @@
         <f>F61*J63</f>
         <v>0.5</v>
       </c>
-      <c r="L63" s="58"/>
+      <c r="L63" s="46"/>
       <c r="M63" s="16">
         <f t="shared" si="18"/>
         <v>0.33333333333333331</v>
@@ -6503,27 +6797,27 @@
         <f t="shared" si="19"/>
         <v>0.33333333333333326</v>
       </c>
-      <c r="O63" s="54"/>
+      <c r="O63" s="40"/>
     </row>
     <row r="64" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A64" s="49"/>
-      <c r="B64" s="47" t="s">
+      <c r="A64" s="43"/>
+      <c r="B64" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="C64" s="47"/>
+      <c r="C64" s="42"/>
       <c r="D64" s="44" t="s">
         <v>116</v>
       </c>
       <c r="E64" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F64" s="42">
+      <c r="F64" s="45">
         <v>1.9</v>
       </c>
-      <c r="G64" s="42">
-        <v>1</v>
-      </c>
-      <c r="H64" s="42">
+      <c r="G64" s="45">
+        <v>1</v>
+      </c>
+      <c r="H64" s="45">
         <v>2.2000000000000002</v>
       </c>
       <c r="I64" s="1" t="s">
@@ -6545,20 +6839,20 @@
         <f>K64/K17</f>
         <v>0.72380952380952379</v>
       </c>
-      <c r="O64" s="54">
+      <c r="O64" s="40">
         <f>SUM(N64:N65)</f>
         <v>1.0495238095238095</v>
       </c>
     </row>
     <row r="65" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A65" s="49"/>
-      <c r="B65" s="49"/>
-      <c r="C65" s="47"/>
+      <c r="A65" s="43"/>
+      <c r="B65" s="43"/>
+      <c r="C65" s="42"/>
       <c r="D65" s="44"/>
       <c r="E65" s="44"/>
-      <c r="F65" s="42"/>
-      <c r="G65" s="42"/>
-      <c r="H65" s="42"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="45"/>
+      <c r="H65" s="45"/>
       <c r="I65" s="1" t="s">
         <v>43</v>
       </c>
@@ -6577,27 +6871,27 @@
         <f>K65/K15</f>
         <v>0.32571428571428568</v>
       </c>
-      <c r="O65" s="54"/>
+      <c r="O65" s="40"/>
     </row>
     <row r="66" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A66" s="49"/>
-      <c r="B66" s="47" t="s">
+      <c r="A66" s="43"/>
+      <c r="B66" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="C66" s="47"/>
+      <c r="C66" s="42"/>
       <c r="D66" s="44" t="s">
         <v>116</v>
       </c>
       <c r="E66" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F66" s="42">
+      <c r="F66" s="45">
         <v>1.8</v>
       </c>
-      <c r="G66" s="42">
-        <v>1</v>
-      </c>
-      <c r="H66" s="42">
+      <c r="G66" s="45">
+        <v>1</v>
+      </c>
+      <c r="H66" s="45">
         <v>0.7</v>
       </c>
       <c r="I66" s="1" t="s">
@@ -6619,20 +6913,20 @@
         <f t="shared" ref="N66:N67" si="21">K66/K14</f>
         <v>0.53999999999999992</v>
       </c>
-      <c r="O66" s="54">
+      <c r="O66" s="40">
         <f>SUM(N66:N67)</f>
         <v>1.0028571428571429</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A67" s="49"/>
-      <c r="B67" s="49"/>
-      <c r="C67" s="47"/>
+      <c r="A67" s="43"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="42"/>
       <c r="D67" s="44"/>
       <c r="E67" s="44"/>
-      <c r="F67" s="42"/>
-      <c r="G67" s="42"/>
-      <c r="H67" s="42"/>
+      <c r="F67" s="45"/>
+      <c r="G67" s="45"/>
+      <c r="H67" s="45"/>
       <c r="I67" s="1" t="s">
         <v>43</v>
       </c>
@@ -6651,11 +6945,183 @@
         <f t="shared" si="21"/>
         <v>0.46285714285714291</v>
       </c>
-      <c r="O67" s="54"/>
+      <c r="O67" s="40"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="196">
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="A5:A18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="A25:A67"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="O32:O33"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="O34:O35"/>
+    <mergeCell ref="B36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="O36:O37"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="O38:O39"/>
+    <mergeCell ref="B40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H40:H42"/>
+    <mergeCell ref="L40:L42"/>
+    <mergeCell ref="O40:O42"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="O43:O44"/>
+    <mergeCell ref="B45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="O45:O46"/>
+    <mergeCell ref="B43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="O49:O50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="L53:L54"/>
+    <mergeCell ref="O53:O54"/>
+    <mergeCell ref="B55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="L55:L56"/>
+    <mergeCell ref="O55:O56"/>
+    <mergeCell ref="B53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="O57:O58"/>
+    <mergeCell ref="B59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="L59:L60"/>
+    <mergeCell ref="O59:O60"/>
+    <mergeCell ref="B57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="H57:H58"/>
     <mergeCell ref="O66:O67"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="B66:C67"/>
@@ -6680,178 +7146,6 @@
     <mergeCell ref="G61:G63"/>
     <mergeCell ref="H61:H63"/>
     <mergeCell ref="L57:L58"/>
-    <mergeCell ref="O57:O58"/>
-    <mergeCell ref="B59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="L59:L60"/>
-    <mergeCell ref="O59:O60"/>
-    <mergeCell ref="B57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="L53:L54"/>
-    <mergeCell ref="O53:O54"/>
-    <mergeCell ref="B55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="L55:L56"/>
-    <mergeCell ref="O55:O56"/>
-    <mergeCell ref="B53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="L49:L50"/>
-    <mergeCell ref="O49:O50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="O43:O44"/>
-    <mergeCell ref="B45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="O45:O46"/>
-    <mergeCell ref="B43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="O38:O39"/>
-    <mergeCell ref="B40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="H40:H42"/>
-    <mergeCell ref="L40:L42"/>
-    <mergeCell ref="O40:O42"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="O32:O33"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="O34:O35"/>
-    <mergeCell ref="B36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="O36:O37"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="A25:A67"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="A5:A18"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Even more changes spotted in mined ore ratio
</commit_message>
<xml_diff>
--- a/Detailed Ore Data.xlsx
+++ b/Detailed Ore Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\BetterStone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5419B2-0B08-4F7A-8B33-DC4517357B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CAF966-1302-41E4-80F5-C28768B3A62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" tabRatio="708" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -695,9 +695,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -803,98 +800,101 @@
     <xf numFmtId="10" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1382,11 +1382,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F15:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15.95" customHeight="1"/>
@@ -1403,46 +1403,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27.75" customHeight="1">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1">
-      <c r="C2" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59" t="s">
+      <c r="C2" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59" t="s">
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="74" t="s">
+      <c r="M2" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="N2" s="74"/>
-      <c r="O2" s="75" t="s">
+      <c r="N2" s="50"/>
+      <c r="O2" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="75"/>
+      <c r="P2" s="51"/>
     </row>
     <row r="3" spans="1:18" s="4" customFormat="1" ht="12" customHeight="1">
       <c r="B3" s="4" t="s">
@@ -1475,7 +1475,7 @@
       <c r="K3" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="L3" s="59"/>
+      <c r="L3" s="49"/>
       <c r="M3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1490,28 +1490,28 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="63" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="59">
+      <c r="F4" s="49">
         <v>5</v>
       </c>
-      <c r="G4" s="59">
-        <v>1</v>
-      </c>
-      <c r="H4" s="59">
+      <c r="G4" s="49">
+        <v>1</v>
+      </c>
+      <c r="H4" s="49">
         <v>0.1</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -1520,107 +1520,107 @@
       <c r="J4" s="1">
         <v>1.4</v>
       </c>
-      <c r="K4" s="76">
+      <c r="K4" s="47">
         <f>F$4*J4</f>
         <v>7</v>
       </c>
-      <c r="L4" s="77" t="s">
+      <c r="L4" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
-      <c r="O4" s="59" t="s">
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="59" t="s">
+      <c r="P4" s="49" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A5" s="61"/>
-      <c r="B5" s="69" t="s">
+      <c r="A5" s="63"/>
+      <c r="B5" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
       <c r="I5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="1">
         <v>3</v>
       </c>
-      <c r="K5" s="76">
+      <c r="K5" s="47">
         <f t="shared" ref="K5:K7" si="0">F$4*J5</f>
         <v>15</v>
       </c>
-      <c r="L5" s="77"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
     </row>
     <row r="6" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A6" s="61"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
+      <c r="A6" s="63"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J6" s="1">
         <v>0.24</v>
       </c>
-      <c r="K6" s="76">
+      <c r="K6" s="47">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="L6" s="77"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
     </row>
     <row r="7" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A7" s="61"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="58" t="s">
+      <c r="A7" s="63"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="58"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
       <c r="I7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="J7" s="1">
         <v>0.4</v>
       </c>
-      <c r="K7" s="76">
+      <c r="K7" s="47">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L7" s="77"/>
-      <c r="M7" s="70"/>
-      <c r="N7" s="70"/>
-      <c r="O7" s="59" t="s">
+      <c r="L7" s="55"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="P7" s="59" t="s">
+      <c r="P7" s="49" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A8" s="61"/>
+      <c r="A8" s="63"/>
       <c r="B8" s="7" t="s">
         <v>20</v>
       </c>
@@ -1654,91 +1654,91 @@
       <c r="L8" s="8"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
-      <c r="R8" s="78" t="s">
+      <c r="R8" s="65" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A9" s="61"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="59">
+      <c r="F9" s="49">
         <v>5</v>
       </c>
-      <c r="G9" s="59">
-        <v>1</v>
-      </c>
-      <c r="H9" s="59">
+      <c r="G9" s="49">
+        <v>1</v>
+      </c>
+      <c r="H9" s="49">
         <v>0.05</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="59">
+      <c r="J9" s="49">
         <v>0.7</v>
       </c>
-      <c r="K9" s="59">
+      <c r="K9" s="49">
         <f>F9*J9</f>
         <v>3.5</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="M9" s="70"/>
-      <c r="N9" s="70"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="59"/>
-      <c r="Q9" s="71"/>
-      <c r="R9" s="78"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="64"/>
+      <c r="R9" s="65"/>
     </row>
     <row r="10" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A10" s="61"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="58" t="s">
+      <c r="C10" s="52"/>
+      <c r="D10" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="58"/>
-      <c r="F10" s="59">
+      <c r="E10" s="53"/>
+      <c r="F10" s="49">
         <v>5</v>
       </c>
-      <c r="G10" s="59">
-        <v>1</v>
-      </c>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59" t="s">
+      <c r="G10" s="49">
+        <v>1</v>
+      </c>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
       <c r="L10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="70"/>
-      <c r="N10" s="70"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="71"/>
-      <c r="R10" s="78"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="64"/>
+      <c r="R10" s="65"/>
     </row>
     <row r="11" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A11" s="61"/>
-      <c r="B11" s="69" t="s">
+      <c r="A11" s="63"/>
+      <c r="B11" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="52" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1778,19 +1778,19 @@
       </c>
       <c r="Q11" s="10">
         <f>P11/SUM(P11:P18)</f>
-        <v>0.13993619399024804</v>
+        <v>8.1757565146342179E-2</v>
       </c>
       <c r="R11" s="11" t="str">
         <f t="shared" ref="R11:R18" si="2">IF(Q11&lt;0.115,"More!",IF(Q11&gt;0.135,"Less!","OK!"))</f>
-        <v>Less!</v>
+        <v>More!</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A12" s="61"/>
-      <c r="B12" s="69" t="s">
+      <c r="A12" s="63"/>
+      <c r="B12" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="52" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="Q12" s="10">
         <f>P12/SUM(P11:P18)</f>
-        <v>0.10983956929902873</v>
+        <v>6.4173645763420759E-2</v>
       </c>
       <c r="R12" s="11" t="str">
         <f t="shared" si="2"/>
@@ -1838,11 +1838,11 @@
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A13" s="61"/>
-      <c r="B13" s="69" t="s">
+      <c r="A13" s="63"/>
+      <c r="B13" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="52" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1882,19 +1882,19 @@
       </c>
       <c r="Q13" s="10">
         <f>P13/SUM(P11:P18)</f>
-        <v>0.18942018942018943</v>
+        <v>0.11066853424377718</v>
       </c>
       <c r="R13" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>Less!</v>
+        <v>More!</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A14" s="61"/>
-      <c r="B14" s="69" t="s">
+      <c r="A14" s="63"/>
+      <c r="B14" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="69" t="s">
+      <c r="C14" s="52" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1934,19 +1934,19 @@
       </c>
       <c r="Q14" s="10">
         <f>P14/SUM(P11:P18)</f>
-        <v>0.13951165302516652</v>
+        <v>8.1509527561352824E-2</v>
       </c>
       <c r="R14" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>Less!</v>
+        <v>More!</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A15" s="61"/>
-      <c r="B15" s="69" t="s">
+      <c r="A15" s="63"/>
+      <c r="B15" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="69" t="s">
+      <c r="C15" s="52" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1955,8 +1955,8 @@
       <c r="E15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="12">
-        <v>1.5</v>
+      <c r="F15" s="78">
+        <v>1</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="K15" s="1">
         <f t="shared" si="1"/>
-        <v>0.15000000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="9"/>
@@ -1982,11 +1982,11 @@
       </c>
       <c r="P15" s="10">
         <f>N49+N50+N52+N69</f>
-        <v>3.0173333333333332</v>
+        <v>4.5259999999999998</v>
       </c>
       <c r="Q15" s="10">
         <f>P15/SUM(P11:P18)</f>
-        <v>0.13186575348737511</v>
+        <v>0.11556362893577285</v>
       </c>
       <c r="R15" s="11" t="str">
         <f t="shared" si="2"/>
@@ -1994,11 +1994,11 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A16" s="61"/>
-      <c r="B16" s="69" t="s">
+      <c r="A16" s="63"/>
+      <c r="B16" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="69" t="s">
+      <c r="C16" s="52" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -2007,8 +2007,8 @@
       <c r="E16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="12">
-        <v>3.5</v>
+      <c r="F16" s="78">
+        <v>1</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -2024,7 +2024,7 @@
       </c>
       <c r="K16" s="1">
         <f t="shared" si="1"/>
-        <v>3.5000000000000003E-2</v>
+        <v>0.01</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="9"/>
@@ -2034,23 +2034,23 @@
       </c>
       <c r="P16" s="10">
         <f>N53+N41+N30+N68+N70</f>
-        <v>2.6542857142857144</v>
+        <v>9.2900000000000009</v>
       </c>
       <c r="Q16" s="10">
         <f>P16/SUM(P11:P18)</f>
-        <v>0.11599957545903491</v>
+        <v>0.2372041787037848</v>
       </c>
       <c r="R16" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>OK!</v>
+        <v>Less!</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A17" s="61"/>
-      <c r="B17" s="69" t="s">
+      <c r="A17" s="63"/>
+      <c r="B17" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="52" t="s">
         <v>40</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -2060,7 +2060,7 @@
         <v>17</v>
       </c>
       <c r="F17" s="1">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="G17" s="1">
         <v>1</v>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="K17" s="1">
         <f t="shared" si="1"/>
-        <v>8.0000000000000002E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="L17" s="8"/>
       <c r="M17" s="9"/>
@@ -2086,11 +2086,11 @@
       </c>
       <c r="P17" s="10">
         <f>N33+N45+N54</f>
-        <v>2.2750000000000004</v>
+        <v>3.6400000000000006</v>
       </c>
       <c r="Q17" s="10">
         <f>P17/SUM(P11:P18)</f>
-        <v>9.9423748072396734E-2</v>
+        <v>9.2941142140126665E-2</v>
       </c>
       <c r="R17" s="11" t="str">
         <f t="shared" si="2"/>
@@ -2098,11 +2098,11 @@
       </c>
     </row>
     <row r="18" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A18" s="61"/>
-      <c r="B18" s="69" t="s">
+      <c r="A18" s="63"/>
+      <c r="B18" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="69" t="s">
+      <c r="C18" s="52" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -2112,7 +2112,7 @@
         <v>17</v>
       </c>
       <c r="F18" s="1">
-        <v>1.5</v>
+        <v>0.3</v>
       </c>
       <c r="G18" s="1">
         <v>1</v>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="K18" s="1">
         <f t="shared" si="1"/>
-        <v>1.4999999999999999E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="9"/>
@@ -2138,23 +2138,23 @@
       </c>
       <c r="P18" s="10">
         <f>N34+N55+N67</f>
-        <v>1.6933333333333334</v>
+        <v>8.4666666666666668</v>
       </c>
       <c r="Q18" s="10">
         <f>P18/SUM(P11:P18)</f>
-        <v>7.4003317246560493E-2</v>
+        <v>0.21618177750542278</v>
       </c>
       <c r="R18" s="11" t="str">
         <f t="shared" si="2"/>
-        <v>More!</v>
+        <v>Less!</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A19" s="61"/>
-      <c r="B19" s="69" t="s">
+      <c r="A19" s="63"/>
+      <c r="B19" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="69" t="s">
+      <c r="C19" s="52" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -2172,7 +2172,7 @@
       <c r="H19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="12" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="1">
@@ -2188,46 +2188,46 @@
       <c r="Q19" s="10"/>
     </row>
     <row r="20" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A20" s="72" t="s">
+      <c r="A20" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="44">
+      <c r="F20" s="43">
         <v>2</v>
       </c>
-      <c r="G20" s="44">
-        <v>1</v>
-      </c>
-      <c r="H20" s="44">
+      <c r="G20" s="43">
+        <v>1</v>
+      </c>
+      <c r="H20" s="43">
         <v>0.08</v>
       </c>
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="45">
+      <c r="J20" s="44">
         <v>0.21</v>
       </c>
-      <c r="K20" s="44">
+      <c r="K20" s="43">
         <f t="shared" si="1"/>
         <v>0.42</v>
       </c>
-      <c r="L20" s="46"/>
-      <c r="M20" s="47">
+      <c r="L20" s="45"/>
+      <c r="M20" s="46">
         <f>J20/J4</f>
         <v>0.15</v>
       </c>
-      <c r="N20" s="47">
+      <c r="N20" s="46">
         <f>K20/K4</f>
         <v>0.06</v>
       </c>
@@ -2241,44 +2241,44 @@
       </c>
     </row>
     <row r="21" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A21" s="72"/>
-      <c r="B21" s="50" t="s">
+      <c r="A21" s="56"/>
+      <c r="B21" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="50" t="s">
+      <c r="C21" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="52" t="s">
+      <c r="E21" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="48">
+      <c r="F21" s="61">
         <v>3</v>
       </c>
-      <c r="G21" s="48">
-        <v>1</v>
-      </c>
-      <c r="H21" s="48">
+      <c r="G21" s="61">
+        <v>1</v>
+      </c>
+      <c r="H21" s="61">
         <v>0.06</v>
       </c>
-      <c r="I21" s="41" t="s">
+      <c r="I21" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="J21" s="20">
+      <c r="J21" s="19">
         <v>0.25</v>
       </c>
-      <c r="K21" s="20">
+      <c r="K21" s="19">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="L21" s="67"/>
-      <c r="M21" s="22">
+      <c r="L21" s="66"/>
+      <c r="M21" s="21">
         <f>J21/J4</f>
         <v>0.17857142857142858</v>
       </c>
-      <c r="N21" s="22">
+      <c r="N21" s="21">
         <f>K21/K4</f>
         <v>0.10714285714285714</v>
       </c>
@@ -2292,121 +2292,121 @@
       </c>
     </row>
     <row r="22" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A22" s="72"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="23" t="s">
+      <c r="A22" s="56"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="53"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="42" t="s">
+      <c r="E22" s="60"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="J22" s="24">
+      <c r="J22" s="23">
         <v>0.5</v>
       </c>
-      <c r="K22" s="24">
+      <c r="K22" s="23">
         <f>F21*J22</f>
         <v>1.5</v>
       </c>
-      <c r="L22" s="68"/>
-      <c r="M22" s="26">
+      <c r="L22" s="67"/>
+      <c r="M22" s="25">
         <f>J22/J19</f>
         <v>0.5</v>
       </c>
-      <c r="N22" s="26">
+      <c r="N22" s="25">
         <f>K22/K19</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="O22" s="10"/>
     </row>
     <row r="23" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A23" s="72"/>
-      <c r="B23" s="50" t="s">
+      <c r="A23" s="56"/>
+      <c r="B23" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="50" t="s">
+      <c r="C23" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="52" t="s">
+      <c r="E23" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="48">
+      <c r="F23" s="61">
         <v>5</v>
       </c>
-      <c r="G23" s="48">
-        <v>1</v>
-      </c>
-      <c r="H23" s="48">
+      <c r="G23" s="61">
+        <v>1</v>
+      </c>
+      <c r="H23" s="61">
         <v>0.06</v>
       </c>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="J23" s="20">
+      <c r="J23" s="19">
         <v>0.4</v>
       </c>
-      <c r="K23" s="20">
+      <c r="K23" s="19">
         <f>F23*J23</f>
         <v>2</v>
       </c>
-      <c r="L23" s="67" t="s">
+      <c r="L23" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="M23" s="22">
+      <c r="M23" s="21">
         <f>J23/J9</f>
         <v>0.57142857142857151</v>
       </c>
-      <c r="N23" s="22">
+      <c r="N23" s="21">
         <f>K23/K9</f>
         <v>0.5714285714285714</v>
       </c>
       <c r="O23" s="10"/>
     </row>
     <row r="24" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A24" s="72"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="23" t="s">
+      <c r="A24" s="56"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="53"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="40" t="s">
+      <c r="E24" s="60"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="J24" s="24">
+      <c r="J24" s="23">
         <v>0.5</v>
       </c>
-      <c r="K24" s="24">
+      <c r="K24" s="23">
         <f>F23*J24</f>
         <v>2.5</v>
       </c>
-      <c r="L24" s="68"/>
-      <c r="M24" s="26">
+      <c r="L24" s="67"/>
+      <c r="M24" s="25">
         <f>J24/J19</f>
         <v>0.5</v>
       </c>
-      <c r="N24" s="26">
+      <c r="N24" s="25">
         <f>K24/K19</f>
         <v>0.55555555555555558</v>
       </c>
       <c r="O24" s="10"/>
     </row>
     <row r="25" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A25" s="72"/>
-      <c r="B25" s="14" t="s">
+      <c r="A25" s="56"/>
+      <c r="B25" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>54</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -2435,174 +2435,174 @@
         <v>4.5</v>
       </c>
       <c r="L25" s="8"/>
-      <c r="M25" s="15">
+      <c r="M25" s="14">
         <f>J25/J9</f>
         <v>1.2857142857142858</v>
       </c>
-      <c r="N25" s="15">
+      <c r="N25" s="14">
         <f>K25/K9</f>
         <v>1.2857142857142858</v>
       </c>
       <c r="O25" s="10"/>
     </row>
     <row r="26" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A26" s="61" t="s">
+      <c r="A26" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="52" t="s">
+      <c r="C26" s="57"/>
+      <c r="D26" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="52" t="s">
+      <c r="E26" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="48">
+      <c r="F26" s="61">
         <v>5</v>
       </c>
-      <c r="G26" s="48">
-        <v>1</v>
-      </c>
-      <c r="H26" s="48">
+      <c r="G26" s="61">
+        <v>1</v>
+      </c>
+      <c r="H26" s="61">
         <v>0.32</v>
       </c>
-      <c r="I26" s="20" t="s">
+      <c r="I26" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="J26" s="20">
+      <c r="J26" s="19">
         <v>0.35</v>
       </c>
-      <c r="K26" s="20">
+      <c r="K26" s="19">
         <f t="shared" si="3"/>
         <v>1.75</v>
       </c>
-      <c r="L26" s="29"/>
-      <c r="M26" s="22">
+      <c r="L26" s="28"/>
+      <c r="M26" s="21">
         <f>J26/J9</f>
         <v>0.5</v>
       </c>
-      <c r="N26" s="22">
+      <c r="N26" s="21">
         <f>K26/K9</f>
         <v>0.5</v>
       </c>
-      <c r="O26" s="60">
+      <c r="O26" s="73">
         <f>SUM(N26:N27)</f>
         <v>1.1428571428571428</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A27" s="61"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="24" t="s">
+      <c r="A27" s="63"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="J27" s="24">
+      <c r="J27" s="23">
         <v>0.45</v>
       </c>
-      <c r="K27" s="24">
+      <c r="K27" s="23">
         <f>F26*J27</f>
         <v>2.25</v>
       </c>
-      <c r="L27" s="30"/>
-      <c r="M27" s="26">
+      <c r="L27" s="29"/>
+      <c r="M27" s="25">
         <f>J27/J14</f>
         <v>0.6428571428571429</v>
       </c>
-      <c r="N27" s="26">
+      <c r="N27" s="25">
         <f>K27/K14</f>
         <v>0.6428571428571429</v>
       </c>
-      <c r="O27" s="55"/>
+      <c r="O27" s="74"/>
     </row>
     <row r="28" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A28" s="61"/>
-      <c r="B28" s="50" t="s">
+      <c r="A28" s="63"/>
+      <c r="B28" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="52" t="s">
+      <c r="C28" s="57"/>
+      <c r="D28" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="52" t="s">
+      <c r="E28" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="F28" s="48">
+      <c r="F28" s="61">
         <v>7</v>
       </c>
-      <c r="G28" s="48">
-        <v>1</v>
-      </c>
-      <c r="H28" s="48">
+      <c r="G28" s="61">
+        <v>1</v>
+      </c>
+      <c r="H28" s="61">
         <v>1.2</v>
       </c>
-      <c r="I28" s="20" t="s">
+      <c r="I28" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J28" s="20">
+      <c r="J28" s="19">
         <v>0.4</v>
       </c>
-      <c r="K28" s="20">
+      <c r="K28" s="19">
         <f t="shared" ref="K28:K34" si="4">F28*J28</f>
         <v>2.8000000000000003</v>
       </c>
-      <c r="L28" s="21"/>
-      <c r="M28" s="22">
+      <c r="L28" s="20"/>
+      <c r="M28" s="21">
         <f>J28/J11</f>
         <v>1</v>
       </c>
-      <c r="N28" s="22">
+      <c r="N28" s="21">
         <f>K28/K11</f>
         <v>1.4000000000000001</v>
       </c>
-      <c r="O28" s="60">
+      <c r="O28" s="73">
         <f>SUM(N28:N29)</f>
         <v>1.6333333333333335</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A29" s="61"/>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="24" t="s">
+      <c r="A29" s="63"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="J29" s="24">
+      <c r="J29" s="23">
         <v>0.15</v>
       </c>
-      <c r="K29" s="24">
+      <c r="K29" s="23">
         <f>F28*J29</f>
         <v>1.05</v>
       </c>
-      <c r="L29" s="31"/>
-      <c r="M29" s="26">
+      <c r="L29" s="30"/>
+      <c r="M29" s="25">
         <f>J29/J19</f>
         <v>0.15</v>
       </c>
-      <c r="N29" s="26">
+      <c r="N29" s="25">
         <f>K29/K19</f>
         <v>0.23333333333333334</v>
       </c>
-      <c r="O29" s="55"/>
+      <c r="O29" s="74"/>
     </row>
     <row r="30" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A30" s="61"/>
-      <c r="B30" s="56" t="s">
+      <c r="A30" s="63"/>
+      <c r="B30" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="56"/>
+      <c r="C30" s="68"/>
       <c r="D30" s="2" t="s">
         <v>16</v>
       </c>
@@ -2631,70 +2631,70 @@
       <c r="L30" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="M30" s="15">
+      <c r="M30" s="14">
         <f>J30/J16</f>
         <v>0.6</v>
       </c>
-      <c r="N30" s="15">
+      <c r="N30" s="14">
         <f>K30/K16</f>
-        <v>1.1828571428571428</v>
-      </c>
-      <c r="O30" s="16">
+        <v>4.1400000000000006</v>
+      </c>
+      <c r="O30" s="15">
         <f t="shared" ref="O30:O33" si="5">N30</f>
-        <v>1.1828571428571428</v>
+        <v>4.1400000000000006</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A31" s="61"/>
-      <c r="B31" s="62" t="s">
+      <c r="A31" s="63"/>
+      <c r="B31" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="62"/>
-      <c r="D31" s="33" t="s">
+      <c r="C31" s="69"/>
+      <c r="D31" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="34">
+      <c r="F31" s="33">
         <v>8.8000000000000007</v>
       </c>
-      <c r="G31" s="34">
-        <v>1</v>
-      </c>
-      <c r="H31" s="34">
+      <c r="G31" s="33">
+        <v>1</v>
+      </c>
+      <c r="H31" s="33">
         <v>0.32</v>
       </c>
-      <c r="I31" s="34" t="s">
+      <c r="I31" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="J31" s="34">
+      <c r="J31" s="33">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="K31" s="34">
+      <c r="K31" s="33">
         <f t="shared" si="4"/>
         <v>6.1600000000000009E-2</v>
       </c>
-      <c r="L31" s="35"/>
-      <c r="M31" s="36">
+      <c r="L31" s="34"/>
+      <c r="M31" s="35">
         <f>J31/J13</f>
         <v>1</v>
       </c>
-      <c r="N31" s="36">
+      <c r="N31" s="35">
         <f>K31/K13</f>
         <v>1.76</v>
       </c>
-      <c r="O31" s="37">
+      <c r="O31" s="36">
         <f t="shared" si="5"/>
         <v>1.76</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.95" customHeight="1">
-      <c r="A32" s="61"/>
-      <c r="B32" s="56" t="s">
+      <c r="A32" s="63"/>
+      <c r="B32" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="56"/>
+      <c r="C32" s="68"/>
       <c r="D32" s="2" t="s">
         <v>67</v>
       </c>
@@ -2721,85 +2721,85 @@
         <v>1.62</v>
       </c>
       <c r="L32" s="8"/>
-      <c r="M32" s="15">
+      <c r="M32" s="14">
         <f>J32/J12</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="N32" s="15">
+      <c r="N32" s="14">
         <f>K32/K12</f>
         <v>1.0799999999999998</v>
       </c>
-      <c r="O32" s="16">
+      <c r="O32" s="15">
         <f t="shared" si="5"/>
         <v>1.0799999999999998</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A33" s="61"/>
-      <c r="B33" s="62" t="s">
+      <c r="A33" s="63"/>
+      <c r="B33" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="33" t="s">
+      <c r="C33" s="69"/>
+      <c r="D33" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="33" t="s">
+      <c r="E33" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="34">
+      <c r="F33" s="33">
         <v>2.7</v>
       </c>
-      <c r="G33" s="34">
-        <v>1</v>
-      </c>
-      <c r="H33" s="34">
+      <c r="G33" s="33">
+        <v>1</v>
+      </c>
+      <c r="H33" s="33">
         <v>2.8</v>
       </c>
-      <c r="I33" s="34" t="s">
+      <c r="I33" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="J33" s="34">
+      <c r="J33" s="33">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K33" s="34">
+      <c r="K33" s="33">
         <f t="shared" si="4"/>
         <v>8.1000000000000013E-3</v>
       </c>
-      <c r="L33" s="35" t="s">
+      <c r="L33" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="M33" s="36">
+      <c r="M33" s="35">
         <f t="shared" ref="M33:N35" si="6">J33/J17</f>
         <v>0.6</v>
       </c>
-      <c r="N33" s="36">
+      <c r="N33" s="35">
         <f t="shared" si="6"/>
-        <v>1.0125000000000002</v>
-      </c>
-      <c r="O33" s="37">
+        <v>1.6200000000000003</v>
+      </c>
+      <c r="O33" s="36">
         <f t="shared" si="5"/>
-        <v>1.0125000000000002</v>
+        <v>1.6200000000000003</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A34" s="61"/>
-      <c r="B34" s="56" t="s">
+      <c r="A34" s="63"/>
+      <c r="B34" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="56"/>
-      <c r="D34" s="66" t="s">
+      <c r="C34" s="68"/>
+      <c r="D34" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="E34" s="66" t="s">
+      <c r="E34" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="F34" s="59">
+      <c r="F34" s="49">
         <v>3.5</v>
       </c>
-      <c r="G34" s="59">
-        <v>1</v>
-      </c>
-      <c r="H34" s="59">
+      <c r="G34" s="49">
+        <v>1</v>
+      </c>
+      <c r="H34" s="49">
         <v>3.1</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -2812,31 +2812,31 @@
         <f t="shared" si="4"/>
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="L34" s="65" t="s">
+      <c r="L34" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="M34" s="15">
+      <c r="M34" s="14">
         <f t="shared" si="6"/>
         <v>0.2</v>
       </c>
-      <c r="N34" s="15">
+      <c r="N34" s="14">
         <f t="shared" si="6"/>
-        <v>0.46666666666666667</v>
-      </c>
-      <c r="O34" s="54">
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="O34" s="72">
         <f>SUM(N34:N35)</f>
-        <v>0.91155555555555567</v>
+        <v>2.7782222222222224</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A35" s="61"/>
-      <c r="B35" s="61"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="66"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="59"/>
-      <c r="H35" s="59"/>
+      <c r="A35" s="63"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
       <c r="I35" s="1" t="s">
         <v>51</v>
       </c>
@@ -2847,111 +2847,111 @@
         <f>F34*J35</f>
         <v>2.0020000000000002</v>
       </c>
-      <c r="L35" s="65"/>
-      <c r="M35" s="15">
+      <c r="L35" s="71"/>
+      <c r="M35" s="14">
         <f t="shared" si="6"/>
         <v>0.57200000000000006</v>
       </c>
-      <c r="N35" s="15">
+      <c r="N35" s="14">
         <f t="shared" si="6"/>
         <v>0.44488888888888894</v>
       </c>
-      <c r="O35" s="54"/>
+      <c r="O35" s="72"/>
     </row>
     <row r="36" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A36" s="61"/>
-      <c r="B36" s="50" t="s">
+      <c r="A36" s="63"/>
+      <c r="B36" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="50"/>
-      <c r="D36" s="63" t="s">
+      <c r="C36" s="57"/>
+      <c r="D36" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="E36" s="63" t="s">
+      <c r="E36" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="F36" s="48">
+      <c r="F36" s="61">
         <v>5</v>
       </c>
-      <c r="G36" s="48">
-        <v>1</v>
-      </c>
-      <c r="H36" s="48">
+      <c r="G36" s="61">
+        <v>1</v>
+      </c>
+      <c r="H36" s="61">
         <v>1.3</v>
       </c>
-      <c r="I36" s="20" t="s">
+      <c r="I36" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="J36" s="20">
+      <c r="J36" s="19">
         <v>0.23400000000000001</v>
       </c>
-      <c r="K36" s="20">
+      <c r="K36" s="19">
         <f>F36*J36</f>
         <v>1.1700000000000002</v>
       </c>
-      <c r="L36" s="29"/>
-      <c r="M36" s="22">
+      <c r="L36" s="28"/>
+      <c r="M36" s="21">
         <f>J36/J9</f>
         <v>0.33428571428571435</v>
       </c>
-      <c r="N36" s="22">
+      <c r="N36" s="21">
         <f>K36/K9</f>
         <v>0.33428571428571435</v>
       </c>
-      <c r="O36" s="60">
+      <c r="O36" s="73">
         <f>SUM(N36:N37)</f>
         <v>1.0009523809523808</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A37" s="61"/>
-      <c r="B37" s="51"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="24" t="s">
+      <c r="A37" s="63"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="J37" s="24">
+      <c r="J37" s="23">
         <v>0.2</v>
       </c>
-      <c r="K37" s="24">
+      <c r="K37" s="23">
         <f>F36*J37</f>
         <v>1</v>
       </c>
-      <c r="L37" s="30"/>
-      <c r="M37" s="26">
+      <c r="L37" s="29"/>
+      <c r="M37" s="25">
         <f>J37/J12</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="N37" s="26">
+      <c r="N37" s="25">
         <f>K37/K12</f>
         <v>0.66666666666666652</v>
       </c>
-      <c r="O37" s="55"/>
+      <c r="O37" s="74"/>
     </row>
     <row r="38" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A38" s="61"/>
-      <c r="B38" s="56" t="s">
+      <c r="A38" s="63"/>
+      <c r="B38" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="56"/>
-      <c r="D38" s="66" t="s">
+      <c r="C38" s="68"/>
+      <c r="D38" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="66" t="s">
+      <c r="E38" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="F38" s="59">
+      <c r="F38" s="49">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G38" s="59">
-        <v>1</v>
-      </c>
-      <c r="H38" s="59">
+      <c r="G38" s="49">
+        <v>1</v>
+      </c>
+      <c r="H38" s="49">
         <v>0.5</v>
       </c>
       <c r="I38" s="1" t="s">
@@ -2964,29 +2964,29 @@
         <f>F38*J38</f>
         <v>2.8519999999999999</v>
       </c>
-      <c r="L38" s="17"/>
-      <c r="M38" s="15">
+      <c r="L38" s="16"/>
+      <c r="M38" s="14">
         <f>J38/J14</f>
         <v>0.88571428571428579</v>
       </c>
-      <c r="N38" s="15">
+      <c r="N38" s="14">
         <f>K38/K14</f>
         <v>0.81485714285714284</v>
       </c>
-      <c r="O38" s="54">
+      <c r="O38" s="72">
         <f>SUM(N38:N39)</f>
         <v>1.1521904761904762</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A39" s="61"/>
-      <c r="B39" s="61"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="59"/>
-      <c r="H39" s="59"/>
+      <c r="A39" s="63"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
       <c r="I39" s="1" t="s">
         <v>51</v>
       </c>
@@ -2997,111 +2997,111 @@
         <f>F38*J39</f>
         <v>1.518</v>
       </c>
-      <c r="L39" s="17"/>
-      <c r="M39" s="15">
+      <c r="L39" s="16"/>
+      <c r="M39" s="14">
         <f>J39/J19</f>
         <v>0.33</v>
       </c>
-      <c r="N39" s="15">
+      <c r="N39" s="14">
         <f>K39/K19</f>
         <v>0.33733333333333332</v>
       </c>
-      <c r="O39" s="54"/>
+      <c r="O39" s="72"/>
     </row>
     <row r="40" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A40" s="61"/>
-      <c r="B40" s="50" t="s">
+      <c r="A40" s="63"/>
+      <c r="B40" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="50"/>
-      <c r="D40" s="63" t="s">
+      <c r="C40" s="57"/>
+      <c r="D40" s="75" t="s">
         <v>79</v>
       </c>
-      <c r="E40" s="63" t="s">
+      <c r="E40" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="F40" s="48">
+      <c r="F40" s="61">
         <v>5.2</v>
       </c>
-      <c r="G40" s="48">
-        <v>1</v>
-      </c>
-      <c r="H40" s="48">
+      <c r="G40" s="61">
+        <v>1</v>
+      </c>
+      <c r="H40" s="61">
         <v>0.25</v>
       </c>
-      <c r="I40" s="20" t="s">
+      <c r="I40" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="J40" s="20">
+      <c r="J40" s="19">
         <v>0.55000000000000004</v>
       </c>
-      <c r="K40" s="20">
+      <c r="K40" s="19">
         <f>F40*J40</f>
         <v>2.8600000000000003</v>
       </c>
-      <c r="L40" s="38"/>
-      <c r="M40" s="22">
+      <c r="L40" s="37"/>
+      <c r="M40" s="21">
         <f>J40/J9</f>
         <v>0.78571428571428581</v>
       </c>
-      <c r="N40" s="22">
+      <c r="N40" s="21">
         <f>K40/K9</f>
         <v>0.81714285714285728</v>
       </c>
-      <c r="O40" s="60">
+      <c r="O40" s="73">
         <f>SUM(N40:N41)</f>
-        <v>1.1142857142857143</v>
+        <v>1.8571428571428572</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A41" s="61"/>
-      <c r="B41" s="57"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="64"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="49"/>
-      <c r="H41" s="49"/>
-      <c r="I41" s="24" t="s">
+      <c r="A41" s="63"/>
+      <c r="B41" s="77"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="62"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="62"/>
+      <c r="I41" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="J41" s="24">
+      <c r="J41" s="23">
         <v>2E-3</v>
       </c>
-      <c r="K41" s="24">
+      <c r="K41" s="23">
         <f>F40*J41</f>
         <v>1.0400000000000001E-2</v>
       </c>
-      <c r="L41" s="39"/>
-      <c r="M41" s="26">
+      <c r="L41" s="38"/>
+      <c r="M41" s="25">
         <f>J41/J16</f>
         <v>0.2</v>
       </c>
-      <c r="N41" s="26">
+      <c r="N41" s="25">
         <f>K41/K16</f>
-        <v>0.29714285714285715</v>
-      </c>
-      <c r="O41" s="55"/>
+        <v>1.04</v>
+      </c>
+      <c r="O41" s="74"/>
     </row>
     <row r="42" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A42" s="61"/>
-      <c r="B42" s="56" t="s">
+      <c r="A42" s="63"/>
+      <c r="B42" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="56"/>
-      <c r="D42" s="58" t="s">
+      <c r="C42" s="68"/>
+      <c r="D42" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="58" t="s">
+      <c r="E42" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="F42" s="59">
+      <c r="F42" s="49">
         <v>5</v>
       </c>
-      <c r="G42" s="59">
-        <v>1</v>
-      </c>
-      <c r="H42" s="59">
+      <c r="G42" s="49">
+        <v>1</v>
+      </c>
+      <c r="H42" s="49">
         <v>1.9</v>
       </c>
       <c r="I42" s="1" t="s">
@@ -3114,31 +3114,31 @@
         <f>F42*J42</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="L42" s="17" t="s">
+      <c r="L42" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="M42" s="15">
+      <c r="M42" s="14">
         <f>J42/J14</f>
         <v>0.25714285714285717</v>
       </c>
-      <c r="N42" s="15">
+      <c r="N42" s="14">
         <f>K42/K14</f>
         <v>0.25714285714285712</v>
       </c>
-      <c r="O42" s="54">
+      <c r="O42" s="72">
         <f>SUM(N42:N44)</f>
         <v>1.7888888888888888</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A43" s="61"/>
-      <c r="B43" s="61"/>
-      <c r="C43" s="56"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="59"/>
-      <c r="H43" s="59"/>
+      <c r="A43" s="63"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
       <c r="I43" s="1" t="s">
         <v>32</v>
       </c>
@@ -3149,26 +3149,26 @@
         <f>F42*J43</f>
         <v>0.04</v>
       </c>
-      <c r="L43" s="17"/>
-      <c r="M43" s="15">
+      <c r="L43" s="16"/>
+      <c r="M43" s="14">
         <f>J43/J13</f>
         <v>1.1428571428571428</v>
       </c>
-      <c r="N43" s="15">
+      <c r="N43" s="14">
         <f>K43/K13</f>
         <v>1.1428571428571428</v>
       </c>
-      <c r="O43" s="54"/>
+      <c r="O43" s="72"/>
     </row>
     <row r="44" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A44" s="61"/>
-      <c r="B44" s="61"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="59"/>
+      <c r="A44" s="63"/>
+      <c r="B44" s="63"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
       <c r="I44" s="1" t="s">
         <v>51</v>
       </c>
@@ -3180,172 +3180,172 @@
         <v>1.75</v>
       </c>
       <c r="L44" s="1"/>
-      <c r="M44" s="15">
+      <c r="M44" s="14">
         <f>J44/J19</f>
         <v>0.35</v>
       </c>
-      <c r="N44" s="15">
+      <c r="N44" s="14">
         <f>K44/K19</f>
         <v>0.3888888888888889</v>
       </c>
-      <c r="O44" s="54"/>
+      <c r="O44" s="72"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A45" s="61"/>
-      <c r="B45" s="50" t="s">
+      <c r="A45" s="63"/>
+      <c r="B45" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="C45" s="50"/>
-      <c r="D45" s="63" t="s">
+      <c r="C45" s="57"/>
+      <c r="D45" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="E45" s="63" t="s">
+      <c r="E45" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="F45" s="48">
+      <c r="F45" s="61">
         <v>1.9</v>
       </c>
-      <c r="G45" s="48">
-        <v>1</v>
-      </c>
-      <c r="H45" s="48">
+      <c r="G45" s="61">
+        <v>1</v>
+      </c>
+      <c r="H45" s="61">
         <v>3.2</v>
       </c>
-      <c r="I45" s="20" t="s">
+      <c r="I45" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="J45" s="20">
+      <c r="J45" s="19">
         <v>2E-3</v>
       </c>
-      <c r="K45" s="20">
+      <c r="K45" s="19">
         <f>F45*J45</f>
         <v>3.8E-3</v>
       </c>
-      <c r="L45" s="29"/>
-      <c r="M45" s="22">
+      <c r="L45" s="28"/>
+      <c r="M45" s="21">
         <f>J45/J17</f>
         <v>0.4</v>
       </c>
-      <c r="N45" s="22">
+      <c r="N45" s="21">
         <f>K45/K17</f>
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="O45" s="60">
+        <v>0.76</v>
+      </c>
+      <c r="O45" s="73">
         <f>SUM(N45:N46)</f>
-        <v>0.81699999999999995</v>
+        <v>1.1019999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A46" s="61"/>
-      <c r="B46" s="57"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="49"/>
-      <c r="H46" s="49"/>
-      <c r="I46" s="24" t="s">
+      <c r="A46" s="63"/>
+      <c r="B46" s="77"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="76"/>
+      <c r="F46" s="62"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="62"/>
+      <c r="I46" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="J46" s="24">
+      <c r="J46" s="23">
         <v>0.36</v>
       </c>
-      <c r="K46" s="24">
+      <c r="K46" s="23">
         <f>F45*J46</f>
         <v>0.68399999999999994</v>
       </c>
-      <c r="L46" s="30"/>
-      <c r="M46" s="26">
+      <c r="L46" s="29"/>
+      <c r="M46" s="25">
         <f>J46/J11</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="N46" s="26">
+      <c r="N46" s="25">
         <f>K46/K11</f>
         <v>0.34199999999999997</v>
       </c>
-      <c r="O46" s="55"/>
+      <c r="O46" s="74"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A47" s="61"/>
-      <c r="B47" s="50" t="s">
+      <c r="A47" s="63"/>
+      <c r="B47" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="50"/>
-      <c r="D47" s="63" t="s">
+      <c r="C47" s="57"/>
+      <c r="D47" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="E47" s="63" t="s">
+      <c r="E47" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="F47" s="48">
+      <c r="F47" s="61">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G47" s="48">
-        <v>1</v>
-      </c>
-      <c r="H47" s="48">
+      <c r="G47" s="61">
+        <v>1</v>
+      </c>
+      <c r="H47" s="61">
         <v>0.9</v>
       </c>
-      <c r="I47" s="20" t="s">
+      <c r="I47" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="J47" s="20">
+      <c r="J47" s="19">
         <v>0.49</v>
       </c>
-      <c r="K47" s="20">
+      <c r="K47" s="19">
         <f>F47*J47</f>
         <v>2.0089999999999999</v>
       </c>
-      <c r="L47" s="29"/>
-      <c r="M47" s="22">
+      <c r="L47" s="28"/>
+      <c r="M47" s="21">
         <f>J47/J14</f>
         <v>0.70000000000000007</v>
       </c>
-      <c r="N47" s="22">
+      <c r="N47" s="21">
         <f>K47/K14</f>
         <v>0.57399999999999995</v>
       </c>
-      <c r="O47" s="60">
+      <c r="O47" s="73">
         <f>SUM(N47:N48)</f>
         <v>1.5944444444444441</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A48" s="61"/>
-      <c r="B48" s="57"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="64"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="49"/>
-      <c r="I48" s="24" t="s">
+      <c r="A48" s="63"/>
+      <c r="B48" s="77"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="76"/>
+      <c r="F48" s="62"/>
+      <c r="G48" s="62"/>
+      <c r="H48" s="62"/>
+      <c r="I48" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="J48" s="24">
+      <c r="J48" s="23">
         <v>1.1200000000000001</v>
       </c>
-      <c r="K48" s="24">
+      <c r="K48" s="23">
         <f>F47*J48</f>
         <v>4.5919999999999996</v>
       </c>
-      <c r="L48" s="30"/>
-      <c r="M48" s="26">
+      <c r="L48" s="29"/>
+      <c r="M48" s="25">
         <f>J48/J19</f>
         <v>1.1200000000000001</v>
       </c>
-      <c r="N48" s="26">
+      <c r="N48" s="25">
         <f>K48/K19</f>
         <v>1.0204444444444443</v>
       </c>
-      <c r="O48" s="55"/>
+      <c r="O48" s="74"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A49" s="61"/>
-      <c r="B49" s="56" t="s">
+      <c r="A49" s="63"/>
+      <c r="B49" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="C49" s="56"/>
+      <c r="C49" s="68"/>
       <c r="D49" s="2" t="s">
         <v>88</v>
       </c>
@@ -3374,115 +3374,115 @@
       <c r="L49" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="M49" s="15">
+      <c r="M49" s="14">
         <f>J49/J15</f>
         <v>0.35000000000000003</v>
       </c>
-      <c r="N49" s="15">
+      <c r="N49" s="14">
         <f>K49/K15</f>
-        <v>1.0033333333333332</v>
-      </c>
-      <c r="O49" s="16">
+        <v>1.5049999999999999</v>
+      </c>
+      <c r="O49" s="15">
         <f t="shared" ref="O49" si="8">N49</f>
-        <v>1.0033333333333332</v>
+        <v>1.5049999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A50" s="61"/>
-      <c r="B50" s="50" t="s">
+      <c r="A50" s="63"/>
+      <c r="B50" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="C50" s="50"/>
-      <c r="D50" s="52" t="s">
+      <c r="C50" s="57"/>
+      <c r="D50" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="E50" s="52" t="s">
+      <c r="E50" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="F50" s="48">
+      <c r="F50" s="61">
         <v>2.4</v>
       </c>
-      <c r="G50" s="48">
-        <v>1</v>
-      </c>
-      <c r="H50" s="48">
+      <c r="G50" s="61">
+        <v>1</v>
+      </c>
+      <c r="H50" s="61">
         <v>0.8</v>
       </c>
-      <c r="I50" s="20" t="s">
+      <c r="I50" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="J50" s="20">
+      <c r="J50" s="19">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="K50" s="20">
+      <c r="K50" s="19">
         <f>F50*J50</f>
         <v>0.15359999999999999</v>
       </c>
-      <c r="L50" s="21"/>
-      <c r="M50" s="22">
+      <c r="L50" s="20"/>
+      <c r="M50" s="21">
         <f>J50/J15</f>
         <v>0.64</v>
       </c>
-      <c r="N50" s="22">
+      <c r="N50" s="21">
         <f>K50/K15</f>
-        <v>1.0239999999999998</v>
-      </c>
-      <c r="O50" s="60">
+        <v>1.5359999999999998</v>
+      </c>
+      <c r="O50" s="73">
         <f>SUM(N50:N51)</f>
-        <v>1.0250666666666666</v>
+        <v>1.5370666666666666</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A51" s="61"/>
-      <c r="B51" s="51"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="49"/>
-      <c r="H51" s="49"/>
-      <c r="I51" s="24" t="s">
+      <c r="A51" s="63"/>
+      <c r="B51" s="58"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="60"/>
+      <c r="F51" s="62"/>
+      <c r="G51" s="62"/>
+      <c r="H51" s="62"/>
+      <c r="I51" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="J51" s="24">
+      <c r="J51" s="23">
         <v>2E-3</v>
       </c>
-      <c r="K51" s="24">
+      <c r="K51" s="23">
         <f>F50*J51</f>
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="L51" s="31" t="s">
+      <c r="L51" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="M51" s="26">
+      <c r="M51" s="25">
         <f>J51/J19</f>
         <v>2E-3</v>
       </c>
-      <c r="N51" s="26">
+      <c r="N51" s="25">
         <f>K51/K19</f>
         <v>1.0666666666666665E-3</v>
       </c>
-      <c r="O51" s="55"/>
+      <c r="O51" s="74"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A52" s="61"/>
-      <c r="B52" s="56" t="s">
+      <c r="A52" s="63"/>
+      <c r="B52" s="68" t="s">
         <v>92</v>
       </c>
-      <c r="C52" s="56"/>
-      <c r="D52" s="58" t="s">
+      <c r="C52" s="68"/>
+      <c r="D52" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="E52" s="58" t="s">
+      <c r="E52" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="F52" s="59">
+      <c r="F52" s="49">
         <v>1.8</v>
       </c>
-      <c r="G52" s="59">
-        <v>1</v>
-      </c>
-      <c r="H52" s="59">
+      <c r="G52" s="49">
+        <v>1</v>
+      </c>
+      <c r="H52" s="49">
         <v>0.7</v>
       </c>
       <c r="I52" s="1" t="s">
@@ -3495,29 +3495,29 @@
         <f t="shared" si="7"/>
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="L52" s="17"/>
-      <c r="M52" s="15">
+      <c r="L52" s="16"/>
+      <c r="M52" s="14">
         <f t="shared" ref="M52:N55" si="9">J52/J15</f>
         <v>0.44999999999999996</v>
       </c>
-      <c r="N52" s="15">
+      <c r="N52" s="14">
         <f t="shared" si="9"/>
-        <v>0.53999999999999992</v>
-      </c>
-      <c r="O52" s="54">
+        <v>0.80999999999999994</v>
+      </c>
+      <c r="O52" s="72">
         <f>SUM(N52:N53)</f>
-        <v>1.0028571428571429</v>
+        <v>2.4300000000000002</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A53" s="61"/>
-      <c r="B53" s="61"/>
-      <c r="C53" s="56"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="59"/>
-      <c r="G53" s="59"/>
-      <c r="H53" s="59"/>
+      <c r="A53" s="63"/>
+      <c r="B53" s="63"/>
+      <c r="C53" s="68"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="49"/>
       <c r="I53" s="1" t="s">
         <v>38</v>
       </c>
@@ -3528,126 +3528,126 @@
         <f>F52*J53</f>
         <v>1.6200000000000003E-2</v>
       </c>
-      <c r="L53" s="17"/>
-      <c r="M53" s="15">
+      <c r="L53" s="16"/>
+      <c r="M53" s="14">
         <f t="shared" si="9"/>
         <v>0.90000000000000013</v>
       </c>
-      <c r="N53" s="15">
+      <c r="N53" s="14">
         <f t="shared" si="9"/>
-        <v>0.46285714285714291</v>
-      </c>
-      <c r="O53" s="54"/>
+        <v>1.6200000000000003</v>
+      </c>
+      <c r="O53" s="72"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A54" s="61"/>
-      <c r="B54" s="62" t="s">
+      <c r="A54" s="63"/>
+      <c r="B54" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="C54" s="62"/>
-      <c r="D54" s="33" t="s">
+      <c r="C54" s="69"/>
+      <c r="D54" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="33" t="s">
+      <c r="E54" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F54" s="34">
+      <c r="F54" s="33">
         <v>2.1</v>
       </c>
-      <c r="G54" s="34">
-        <v>1</v>
-      </c>
-      <c r="H54" s="34">
+      <c r="G54" s="33">
+        <v>1</v>
+      </c>
+      <c r="H54" s="33">
         <v>3.6</v>
       </c>
-      <c r="I54" s="34" t="s">
+      <c r="I54" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="J54" s="34">
+      <c r="J54" s="33">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K54" s="34">
+      <c r="K54" s="33">
         <f t="shared" ref="K54:K56" si="10">F54*J54</f>
         <v>6.3E-3</v>
       </c>
-      <c r="L54" s="35"/>
-      <c r="M54" s="36">
+      <c r="L54" s="34"/>
+      <c r="M54" s="35">
         <f t="shared" si="9"/>
         <v>0.6</v>
       </c>
-      <c r="N54" s="36">
+      <c r="N54" s="35">
         <f t="shared" si="9"/>
-        <v>0.78749999999999998</v>
-      </c>
-      <c r="O54" s="37">
+        <v>1.26</v>
+      </c>
+      <c r="O54" s="36">
         <f t="shared" ref="O54:O55" si="11">N54</f>
-        <v>0.78749999999999998</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A55" s="61"/>
-      <c r="B55" s="62" t="s">
+      <c r="A55" s="63"/>
+      <c r="B55" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="62"/>
-      <c r="D55" s="33" t="s">
+      <c r="C55" s="69"/>
+      <c r="D55" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="E55" s="33" t="s">
+      <c r="E55" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F55" s="34">
+      <c r="F55" s="33">
         <v>2.7</v>
       </c>
-      <c r="G55" s="34">
-        <v>1</v>
-      </c>
-      <c r="H55" s="34">
+      <c r="G55" s="33">
+        <v>1</v>
+      </c>
+      <c r="H55" s="33">
         <v>2.8</v>
       </c>
-      <c r="I55" s="34" t="s">
+      <c r="I55" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="J55" s="34">
+      <c r="J55" s="33">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="K55" s="34">
+      <c r="K55" s="33">
         <f t="shared" si="10"/>
         <v>1.0800000000000001E-2</v>
       </c>
-      <c r="L55" s="35"/>
-      <c r="M55" s="36">
+      <c r="L55" s="34"/>
+      <c r="M55" s="35">
         <f t="shared" si="9"/>
         <v>0.4</v>
       </c>
-      <c r="N55" s="36">
+      <c r="N55" s="35">
         <f t="shared" si="9"/>
-        <v>0.72000000000000008</v>
-      </c>
-      <c r="O55" s="37">
+        <v>3.6</v>
+      </c>
+      <c r="O55" s="36">
         <f t="shared" si="11"/>
-        <v>0.72000000000000008</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A56" s="61"/>
-      <c r="B56" s="56" t="s">
+      <c r="A56" s="63"/>
+      <c r="B56" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="C56" s="56"/>
-      <c r="D56" s="58" t="s">
+      <c r="C56" s="68"/>
+      <c r="D56" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="E56" s="58" t="s">
+      <c r="E56" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="F56" s="59">
+      <c r="F56" s="49">
         <v>6.6</v>
       </c>
-      <c r="G56" s="59">
-        <v>1</v>
-      </c>
-      <c r="H56" s="59">
+      <c r="G56" s="49">
+        <v>1</v>
+      </c>
+      <c r="H56" s="49">
         <v>0.35</v>
       </c>
       <c r="I56" s="1" t="s">
@@ -3660,31 +3660,31 @@
         <f t="shared" si="10"/>
         <v>1.452</v>
       </c>
-      <c r="L56" s="17" t="s">
+      <c r="L56" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="M56" s="15">
+      <c r="M56" s="14">
         <f>J56/J14</f>
         <v>0.31428571428571433</v>
       </c>
-      <c r="N56" s="15">
+      <c r="N56" s="14">
         <f>K56/K14</f>
         <v>0.41485714285714287</v>
       </c>
-      <c r="O56" s="54">
+      <c r="O56" s="72">
         <f>SUM(N56:N57)</f>
         <v>1.3577142857142857</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A57" s="61"/>
-      <c r="B57" s="61"/>
-      <c r="C57" s="56"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="59"/>
-      <c r="G57" s="59"/>
-      <c r="H57" s="59"/>
+      <c r="A57" s="63"/>
+      <c r="B57" s="63"/>
+      <c r="C57" s="68"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="53"/>
+      <c r="F57" s="49"/>
+      <c r="G57" s="49"/>
+      <c r="H57" s="49"/>
       <c r="I57" s="1" t="s">
         <v>32</v>
       </c>
@@ -3695,111 +3695,111 @@
         <f>F56*J57</f>
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="L57" s="17"/>
-      <c r="M57" s="15">
+      <c r="L57" s="16"/>
+      <c r="M57" s="14">
         <f>J57/J13</f>
         <v>0.7142857142857143</v>
       </c>
-      <c r="N57" s="15">
+      <c r="N57" s="14">
         <f>K57/K13</f>
         <v>0.94285714285714284</v>
       </c>
-      <c r="O57" s="54"/>
+      <c r="O57" s="72"/>
     </row>
     <row r="58" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A58" s="61"/>
-      <c r="B58" s="50" t="s">
+      <c r="A58" s="63"/>
+      <c r="B58" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="50"/>
-      <c r="D58" s="52" t="s">
+      <c r="C58" s="57"/>
+      <c r="D58" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="E58" s="52" t="s">
+      <c r="E58" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="F58" s="48">
+      <c r="F58" s="61">
         <v>5.7</v>
       </c>
-      <c r="G58" s="48">
-        <v>1</v>
-      </c>
-      <c r="H58" s="48">
+      <c r="G58" s="61">
+        <v>1</v>
+      </c>
+      <c r="H58" s="61">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I58" s="20" t="s">
+      <c r="I58" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="J58" s="20">
+      <c r="J58" s="19">
         <v>0.3</v>
       </c>
-      <c r="K58" s="20">
+      <c r="K58" s="19">
         <f>F58*J58</f>
         <v>1.71</v>
       </c>
-      <c r="L58" s="29"/>
-      <c r="M58" s="22">
+      <c r="L58" s="28"/>
+      <c r="M58" s="21">
         <f>J58/J14</f>
         <v>0.4285714285714286</v>
       </c>
-      <c r="N58" s="22">
+      <c r="N58" s="21">
         <f>K58/K14</f>
         <v>0.48857142857142855</v>
       </c>
-      <c r="O58" s="60">
+      <c r="O58" s="73">
         <f>SUM(N58:N59)</f>
         <v>0.97714285714285709</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A59" s="61"/>
-      <c r="B59" s="57"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="53"/>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="49"/>
-      <c r="I59" s="24" t="s">
+      <c r="A59" s="63"/>
+      <c r="B59" s="77"/>
+      <c r="C59" s="58"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="60"/>
+      <c r="F59" s="62"/>
+      <c r="G59" s="62"/>
+      <c r="H59" s="62"/>
+      <c r="I59" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J59" s="24">
+      <c r="J59" s="23">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K59" s="24">
+      <c r="K59" s="23">
         <f>F58*J59</f>
         <v>1.7100000000000001E-2</v>
       </c>
-      <c r="L59" s="30"/>
-      <c r="M59" s="26">
+      <c r="L59" s="29"/>
+      <c r="M59" s="25">
         <f>J59/J13</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="N59" s="26">
+      <c r="N59" s="25">
         <f>K59/K13</f>
         <v>0.48857142857142855</v>
       </c>
-      <c r="O59" s="55"/>
+      <c r="O59" s="74"/>
     </row>
     <row r="60" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A60" s="61"/>
-      <c r="B60" s="56" t="s">
+      <c r="A60" s="63"/>
+      <c r="B60" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="C60" s="56"/>
-      <c r="D60" s="58" t="s">
+      <c r="C60" s="68"/>
+      <c r="D60" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E60" s="58" t="s">
+      <c r="E60" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="F60" s="59">
+      <c r="F60" s="49">
         <v>5</v>
       </c>
-      <c r="G60" s="59">
-        <v>1</v>
-      </c>
-      <c r="H60" s="59">
+      <c r="G60" s="49">
+        <v>1</v>
+      </c>
+      <c r="H60" s="49">
         <v>1.0249999999999999</v>
       </c>
       <c r="I60" s="1" t="s">
@@ -3812,29 +3812,29 @@
         <f>F60*J60</f>
         <v>1.75</v>
       </c>
-      <c r="L60" s="17"/>
-      <c r="M60" s="15">
+      <c r="L60" s="16"/>
+      <c r="M60" s="14">
         <f>J60/J9</f>
         <v>0.5</v>
       </c>
-      <c r="N60" s="15">
+      <c r="N60" s="14">
         <f>K60/K9</f>
         <v>0.5</v>
       </c>
-      <c r="O60" s="54">
+      <c r="O60" s="72">
         <f>SUM(N60:N61)</f>
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A61" s="61"/>
-      <c r="B61" s="61"/>
-      <c r="C61" s="56"/>
-      <c r="D61" s="58"/>
-      <c r="E61" s="58"/>
-      <c r="F61" s="59"/>
-      <c r="G61" s="59"/>
-      <c r="H61" s="59"/>
+      <c r="A61" s="63"/>
+      <c r="B61" s="63"/>
+      <c r="C61" s="68"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="49"/>
       <c r="I61" s="1" t="s">
         <v>28</v>
       </c>
@@ -3845,111 +3845,111 @@
         <f>F60*J61</f>
         <v>1</v>
       </c>
-      <c r="L61" s="17"/>
-      <c r="M61" s="15">
+      <c r="L61" s="16"/>
+      <c r="M61" s="14">
         <f>J61/J11</f>
         <v>0.5</v>
       </c>
-      <c r="N61" s="15">
+      <c r="N61" s="14">
         <f>K61/K11</f>
         <v>0.5</v>
       </c>
-      <c r="O61" s="54"/>
+      <c r="O61" s="72"/>
     </row>
     <row r="62" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A62" s="61"/>
-      <c r="B62" s="50" t="s">
+      <c r="A62" s="63"/>
+      <c r="B62" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="C62" s="50"/>
-      <c r="D62" s="52" t="s">
+      <c r="C62" s="57"/>
+      <c r="D62" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="E62" s="52" t="s">
+      <c r="E62" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="F62" s="48">
+      <c r="F62" s="61">
         <v>5</v>
       </c>
-      <c r="G62" s="48">
-        <v>1</v>
-      </c>
-      <c r="H62" s="48">
+      <c r="G62" s="61">
+        <v>1</v>
+      </c>
+      <c r="H62" s="61">
         <v>0.67200000000000004</v>
       </c>
-      <c r="I62" s="20" t="s">
+      <c r="I62" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J62" s="20">
+      <c r="J62" s="19">
         <v>0.21</v>
       </c>
-      <c r="K62" s="20">
+      <c r="K62" s="19">
         <f>F62*J62</f>
         <v>1.05</v>
       </c>
-      <c r="L62" s="27"/>
-      <c r="M62" s="22">
+      <c r="L62" s="26"/>
+      <c r="M62" s="21">
         <f>J62/J11</f>
         <v>0.52499999999999991</v>
       </c>
-      <c r="N62" s="22">
+      <c r="N62" s="21">
         <f>K62/K11</f>
         <v>0.52500000000000002</v>
       </c>
-      <c r="O62" s="60">
+      <c r="O62" s="73">
         <f>SUM(N62:N63)</f>
         <v>0.95833333333333326</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A63" s="61"/>
-      <c r="B63" s="51"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="53"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="49"/>
-      <c r="G63" s="49"/>
-      <c r="H63" s="49"/>
-      <c r="I63" s="24" t="s">
+      <c r="A63" s="63"/>
+      <c r="B63" s="58"/>
+      <c r="C63" s="58"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="60"/>
+      <c r="F63" s="62"/>
+      <c r="G63" s="62"/>
+      <c r="H63" s="62"/>
+      <c r="I63" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="J63" s="24">
+      <c r="J63" s="23">
         <v>0.13</v>
       </c>
-      <c r="K63" s="24">
+      <c r="K63" s="23">
         <f>F62*J63</f>
         <v>0.65</v>
       </c>
-      <c r="L63" s="28"/>
-      <c r="M63" s="26">
+      <c r="L63" s="27"/>
+      <c r="M63" s="25">
         <f>J63/J12</f>
         <v>0.43333333333333329</v>
       </c>
-      <c r="N63" s="26">
+      <c r="N63" s="25">
         <f>K63/K12</f>
         <v>0.43333333333333329</v>
       </c>
-      <c r="O63" s="55"/>
+      <c r="O63" s="74"/>
     </row>
     <row r="64" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A64" s="61"/>
-      <c r="B64" s="56" t="s">
+      <c r="A64" s="63"/>
+      <c r="B64" s="68" t="s">
         <v>106</v>
       </c>
-      <c r="C64" s="56"/>
-      <c r="D64" s="58" t="s">
+      <c r="C64" s="68"/>
+      <c r="D64" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="E64" s="58" t="s">
+      <c r="E64" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="F64" s="59">
+      <c r="F64" s="49">
         <v>5</v>
       </c>
-      <c r="G64" s="59">
-        <v>1</v>
-      </c>
-      <c r="H64" s="59">
+      <c r="G64" s="49">
+        <v>1</v>
+      </c>
+      <c r="H64" s="49">
         <v>0.67200000000000004</v>
       </c>
       <c r="I64" s="1" t="s">
@@ -3962,29 +3962,29 @@
         <f>F64*J64</f>
         <v>1.42</v>
       </c>
-      <c r="L64" s="18"/>
-      <c r="M64" s="15">
+      <c r="L64" s="17"/>
+      <c r="M64" s="14">
         <f>J64/J9</f>
         <v>0.40571428571428569</v>
       </c>
-      <c r="N64" s="15">
+      <c r="N64" s="14">
         <f>K64/K9</f>
         <v>0.40571428571428569</v>
       </c>
-      <c r="O64" s="54">
+      <c r="O64" s="72">
         <f>SUM(N64:N66)</f>
         <v>1.1740476190476188</v>
       </c>
     </row>
     <row r="65" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A65" s="61"/>
-      <c r="B65" s="56"/>
-      <c r="C65" s="56"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="58"/>
-      <c r="F65" s="59"/>
-      <c r="G65" s="59"/>
-      <c r="H65" s="59"/>
+      <c r="A65" s="63"/>
+      <c r="B65" s="68"/>
+      <c r="C65" s="68"/>
+      <c r="D65" s="53"/>
+      <c r="E65" s="53"/>
+      <c r="F65" s="49"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="49"/>
       <c r="I65" s="1" t="s">
         <v>28</v>
       </c>
@@ -3995,28 +3995,28 @@
         <f>F64*J65</f>
         <v>0.86999999999999988</v>
       </c>
-      <c r="L65" s="18"/>
-      <c r="M65" s="15">
+      <c r="L65" s="17"/>
+      <c r="M65" s="14">
         <f>J65/J11</f>
         <v>0.43499999999999994</v>
       </c>
-      <c r="N65" s="15">
+      <c r="N65" s="14">
         <f>K65/K11</f>
         <v>0.43499999999999994</v>
       </c>
-      <c r="O65" s="54"/>
+      <c r="O65" s="72"/>
     </row>
     <row r="66" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A66" s="61"/>
-      <c r="B66" s="56"/>
-      <c r="C66" s="56"/>
-      <c r="D66" s="58"/>
-      <c r="E66" s="58"/>
-      <c r="F66" s="59"/>
-      <c r="G66" s="59">
-        <v>1</v>
-      </c>
-      <c r="H66" s="59"/>
+      <c r="A66" s="63"/>
+      <c r="B66" s="68"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="53"/>
+      <c r="E66" s="53"/>
+      <c r="F66" s="49"/>
+      <c r="G66" s="49">
+        <v>1</v>
+      </c>
+      <c r="H66" s="49"/>
       <c r="I66" s="1" t="s">
         <v>30</v>
       </c>
@@ -4027,111 +4027,111 @@
         <f>F64*J66</f>
         <v>0.5</v>
       </c>
-      <c r="L66" s="18"/>
-      <c r="M66" s="15">
+      <c r="L66" s="17"/>
+      <c r="M66" s="14">
         <f>J66/J12</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N66" s="15">
+      <c r="N66" s="14">
         <f>K66/K12</f>
         <v>0.33333333333333326</v>
       </c>
-      <c r="O66" s="54"/>
+      <c r="O66" s="72"/>
     </row>
     <row r="67" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A67" s="61"/>
-      <c r="B67" s="50" t="s">
+      <c r="A67" s="63"/>
+      <c r="B67" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="C67" s="50"/>
-      <c r="D67" s="52" t="s">
+      <c r="C67" s="57"/>
+      <c r="D67" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="E67" s="52" t="s">
+      <c r="E67" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="F67" s="48">
+      <c r="F67" s="61">
         <v>1.9</v>
       </c>
-      <c r="G67" s="48">
-        <v>1</v>
-      </c>
-      <c r="H67" s="48">
+      <c r="G67" s="61">
+        <v>1</v>
+      </c>
+      <c r="H67" s="61">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I67" s="20" t="s">
+      <c r="I67" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="J67" s="20">
+      <c r="J67" s="19">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="K67" s="20">
+      <c r="K67" s="19">
         <f>F67*J67</f>
         <v>7.6E-3</v>
       </c>
-      <c r="L67" s="21"/>
-      <c r="M67" s="22">
+      <c r="L67" s="20"/>
+      <c r="M67" s="21">
         <f>J67/J18</f>
         <v>0.4</v>
       </c>
-      <c r="N67" s="22">
+      <c r="N67" s="21">
         <f>K67/K18</f>
-        <v>0.50666666666666671</v>
-      </c>
-      <c r="O67" s="60">
+        <v>2.5333333333333332</v>
+      </c>
+      <c r="O67" s="73">
         <f>SUM(N67:N68)</f>
-        <v>0.83238095238095244</v>
+        <v>3.6733333333333333</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A68" s="61"/>
-      <c r="B68" s="57"/>
-      <c r="C68" s="51"/>
-      <c r="D68" s="53"/>
-      <c r="E68" s="53"/>
-      <c r="F68" s="49"/>
-      <c r="G68" s="49"/>
-      <c r="H68" s="49"/>
-      <c r="I68" s="24" t="s">
+      <c r="A68" s="63"/>
+      <c r="B68" s="77"/>
+      <c r="C68" s="58"/>
+      <c r="D68" s="60"/>
+      <c r="E68" s="60"/>
+      <c r="F68" s="62"/>
+      <c r="G68" s="62"/>
+      <c r="H68" s="62"/>
+      <c r="I68" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="J68" s="24">
+      <c r="J68" s="23">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="K68" s="24">
+      <c r="K68" s="23">
         <f>F67*J68</f>
         <v>1.14E-2</v>
       </c>
-      <c r="L68" s="25"/>
-      <c r="M68" s="26">
+      <c r="L68" s="24"/>
+      <c r="M68" s="25">
         <f>J68/J16</f>
         <v>0.6</v>
       </c>
-      <c r="N68" s="26">
+      <c r="N68" s="25">
         <f>K68/K16</f>
-        <v>0.32571428571428568</v>
-      </c>
-      <c r="O68" s="55"/>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="O68" s="74"/>
     </row>
     <row r="69" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A69" s="61"/>
-      <c r="B69" s="56" t="s">
+      <c r="A69" s="63"/>
+      <c r="B69" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="C69" s="56"/>
-      <c r="D69" s="58" t="s">
+      <c r="C69" s="68"/>
+      <c r="D69" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="E69" s="58" t="s">
+      <c r="E69" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="F69" s="59">
+      <c r="F69" s="49">
         <v>1.5</v>
       </c>
-      <c r="G69" s="59">
-        <v>1</v>
-      </c>
-      <c r="H69" s="59">
+      <c r="G69" s="49">
+        <v>1</v>
+      </c>
+      <c r="H69" s="49">
         <v>0.7</v>
       </c>
       <c r="I69" s="1" t="s">
@@ -4145,52 +4145,221 @@
         <v>6.7500000000000004E-2</v>
       </c>
       <c r="L69" s="8"/>
-      <c r="M69" s="15">
+      <c r="M69" s="14">
         <f>J69/J15</f>
         <v>0.44999999999999996</v>
       </c>
-      <c r="N69" s="15">
+      <c r="N69" s="14">
         <f>K69/K15</f>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="O69" s="54">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="O69" s="72">
         <f>SUM(N69:N70)</f>
-        <v>0.83571428571428563</v>
+        <v>2.0250000000000004</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="15.95" customHeight="1">
-      <c r="A70" s="61"/>
-      <c r="B70" s="57"/>
-      <c r="C70" s="51"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="49"/>
-      <c r="G70" s="49"/>
-      <c r="H70" s="49"/>
-      <c r="I70" s="24" t="s">
+      <c r="A70" s="63"/>
+      <c r="B70" s="77"/>
+      <c r="C70" s="58"/>
+      <c r="D70" s="60"/>
+      <c r="E70" s="60"/>
+      <c r="F70" s="62"/>
+      <c r="G70" s="62"/>
+      <c r="H70" s="62"/>
+      <c r="I70" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="J70" s="24">
+      <c r="J70" s="23">
         <v>9.0000000000000011E-3</v>
       </c>
-      <c r="K70" s="24">
+      <c r="K70" s="23">
         <f>F69*J70</f>
         <v>1.3500000000000002E-2</v>
       </c>
-      <c r="L70" s="25"/>
-      <c r="M70" s="26">
+      <c r="L70" s="24"/>
+      <c r="M70" s="25">
         <f>J70/J16</f>
         <v>0.90000000000000013</v>
       </c>
-      <c r="N70" s="26">
+      <c r="N70" s="25">
         <f>K70/K16</f>
-        <v>0.38571428571428573</v>
-      </c>
-      <c r="O70" s="55"/>
+        <v>1.35</v>
+      </c>
+      <c r="O70" s="74"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="193">
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="B50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="O69:O70"/>
+    <mergeCell ref="B69:C70"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="O64:O66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="G67:G68"/>
+    <mergeCell ref="H67:H68"/>
+    <mergeCell ref="O67:O68"/>
+    <mergeCell ref="B64:C66"/>
+    <mergeCell ref="H64:H66"/>
+    <mergeCell ref="O60:O61"/>
+    <mergeCell ref="B62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="O62:O63"/>
+    <mergeCell ref="B60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="H60:H61"/>
+    <mergeCell ref="O56:O57"/>
+    <mergeCell ref="B58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="B56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="H52:H53"/>
+    <mergeCell ref="O52:O53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="O50:O51"/>
+    <mergeCell ref="O45:O46"/>
+    <mergeCell ref="B47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="O47:O48"/>
+    <mergeCell ref="B45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="B42:C44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="G42:G44"/>
+    <mergeCell ref="H42:H44"/>
+    <mergeCell ref="O42:O44"/>
+    <mergeCell ref="B40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="G64:G66"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="O34:O35"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="O36:O37"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="O38:O39"/>
+    <mergeCell ref="B36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="O40:O41"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="A26:A70"/>
+    <mergeCell ref="B26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="B28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="D64:D66"/>
+    <mergeCell ref="E64:E66"/>
+    <mergeCell ref="F64:F66"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="R8:R10"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="A4:A19"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="I2:K2"/>
@@ -4215,175 +4384,6 @@
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="D4:D7"/>
     <mergeCell ref="E4:E7"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="A4:A19"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="R8:R10"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="A26:A70"/>
-    <mergeCell ref="B26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="B28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="D64:D66"/>
-    <mergeCell ref="E64:E66"/>
-    <mergeCell ref="F64:F66"/>
-    <mergeCell ref="G64:G66"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="O34:O35"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="O36:O37"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="O38:O39"/>
-    <mergeCell ref="B36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="O40:O41"/>
-    <mergeCell ref="B42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="H42:H44"/>
-    <mergeCell ref="O42:O44"/>
-    <mergeCell ref="B40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="O45:O46"/>
-    <mergeCell ref="B47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="O47:O48"/>
-    <mergeCell ref="B45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="H52:H53"/>
-    <mergeCell ref="O52:O53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="O50:O51"/>
-    <mergeCell ref="O56:O57"/>
-    <mergeCell ref="B58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="B56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="O60:O61"/>
-    <mergeCell ref="B62:C63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="O62:O63"/>
-    <mergeCell ref="B60:C61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="H60:H61"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="B50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="H50:H51"/>
-    <mergeCell ref="O69:O70"/>
-    <mergeCell ref="B69:C70"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="H69:H70"/>
-    <mergeCell ref="O64:O66"/>
-    <mergeCell ref="B67:C68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="H67:H68"/>
-    <mergeCell ref="O67:O68"/>
-    <mergeCell ref="B64:C66"/>
-    <mergeCell ref="H64:H66"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>